<commit_message>
Some substring template problems
</commit_message>
<xml_diff>
--- a/Leetcode record for Shiyun.xlsx
+++ b/Leetcode record for Shiyun.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Basic Algorithm" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Record 1'!$A$1:$AE$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Record 1'!$A$1:$AF$128</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="410">
   <si>
     <t>Two Pointers</t>
   </si>
@@ -1747,9 +1747,6 @@
 </t>
   </si>
   <si>
-    <t>Count Numbers with Unique Digits Add to List</t>
-  </si>
-  <si>
     <t>Given a non-negative integer n, count all numbers with unique digits, x, where 0 ≤ x &lt; 10n.
 Example:
 Given n = 2, return 91. (The answer should be the total numbers in the range of 0 ≤ x &lt; 100, excluding [11,22,33,44,55,66,77,88,99]) 
@@ -1792,6 +1789,421 @@
       <t xml:space="preserve">
 The problem is asking for numbers from 0 to 10^n. Hence return f(1) + f(2) + .. + f(n)</t>
     </r>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Moving Average from Data Stream</t>
+  </si>
+  <si>
+    <t>Desgin</t>
+  </si>
+  <si>
+    <t>计算移动平均数
+MovingAverage m = new MovingAverage(3);
+m.next(1) = 1
+m.next(10) = (1 + 10) / 2
+m.next(3) = (1 + 10 + 3) / 3
+m.next(5) = (10 + 3 + 5) / 3</t>
+  </si>
+  <si>
+    <t>注意：
+1. 结果是double，计算时要cast
+2. 需要在class内声明Instance var, 在constructor中initialize, 在方法中被调用
+3. 用list实现queue</t>
+  </si>
+  <si>
+    <t>Corner cases:
+1. empty string input
+2. empty dictionary array
+3. ["a","a"],isUnique("a")</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Assume you have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String[] dictionary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and given a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String word</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, find whether its abbreviation is unique in the dictionary. A word's abbreviation is unique if no other word from the dictionary has the same abbreviation.
+Example: 
+Given dictionary = [ "deer", "door", "cake", "card" ]
+isUnique("dear") -&gt; 
+false
+isUnique("cart") -&gt; 
+true</t>
+    </r>
+  </si>
+  <si>
+    <t>Unique Word Abbreviation</t>
+  </si>
+  <si>
+    <t>Pinterest</t>
+  </si>
+  <si>
+    <t>Is Subsequence</t>
+  </si>
+  <si>
+    <t>List内元素操作：
+list.set(index, value)对， list.get(index)++无法编译，for(int x : list) x++能编译没作用
+另：indexOf比charAt快</t>
+  </si>
+  <si>
+    <t>Suppose a sorted array is rotated at some pivot unknown to you beforehand.
+(i.e., 0 1 2 4 5 6 7 might become 4 5 6 7 0 1 2).
+Find the minimum element.
+You may assume no duplicate exists in the array.</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Binary Search:
+1. Terminate condition:  left &lt; right - 1
+2. 注意别混淆了Index和array[index]</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Given a string s and a string t, check if s is subsequence of t.
+You may assume that there is only lower case English letters in both s and t. t is potentially a very long (length ~= 500,000) string, and s is a short string (&lt;=100).
+A subsequence of a string is a new string which is formed from the original string by deleting some (can be none) of the characters without disturbing the relative positions of the remaining characters. 
+Example 1:
+s = "abc", t = "ahbgdc" //Return true.
+Example 2:
+s = "axc", t = "ahbgdc"//Return false.
+Follow up:
+If there are lots of incoming S, say S1, S2, ... , Sk where k &gt;= 1B, and you want to check one by one to see if T has its subsequence. In this scenario, how would you change your code?</t>
+  </si>
+  <si>
+    <t>H-Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given an array of citations (each citation is a non-negative integer) of a researcher, write a function to compute the researcher's h-index. 
+According to the definition of h-index on Wikipedia: "A scientist has index h if h of his/her N papers have at least h citations each, and the other N − h papers have no more than h citations each." 
+For example, given citations = [3, 0, 6, 1, 5], which means the researcher has 5 papers in total and each of them had received 3, 0, 6, 1, 5 citations respectively. Since the researcher has 3 papers with at least 3 citations each and the remaining two with no more than 3 citations each, his h-index is 3. 
+Note: If there are several possible values for h, the maximum one is taken as the h-index. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">My solution using sort is easy:) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>using extra space would be faster(https://leetcode.com/articles/h-index/)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Time complexity : O(nlogn). Comparison sorting dominates the time complexity.
+Space complexity : O(1). Most libraries using heap sort which costs O(1) extra space in the worst case.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>H-Index II</t>
+  </si>
+  <si>
+    <t>array is sorted</t>
+  </si>
+  <si>
+    <t>Bloomberg
+Google 
+FaceBook</t>
+  </si>
+  <si>
+    <t>If linear search, notice:
+1. &gt; or &lt;
+2. return the smaller one
+3. index of I
+Binary search can be faster, notice
+1. end condition
+2. new value of pointers(a, b or left right)</t>
+  </si>
+  <si>
+    <t>Heaters</t>
+  </si>
+  <si>
+    <t>Given positions of houses and heaters on a horizontal line, find out minimum radius of heaters so that all houses could be covered by those heaters.
+So, your input will be the positions of houses and heaters seperately, and your expected output will be the minimum radius standard of heaters.
+Note:
+Numbers of houses and heaters you are given are non-negative and will not exceed 25000.
+Positions of houses and heaters you are given are non-negative and will not exceed 10^9.
+As long as a house is in the heaters' warm radius range, it can be warmed.
+All the heaters follow your radius standard and the warm radius will the same.
+Example 1:
+Input: [1,2,3],[2]//Output: 1
+Example 2:
+Input: [1,2,3,4],[1,4]//Output: 1</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Two pointers: pay attention to the increase condition for the 2nd pointer
+2. Arrays.binarySearch() 
+public static</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> int binarySearch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Object[] a,
+               int fromIndex, //optional
+               int toIndex,//optional
+               Object key)
+Parameters:
+a - the array to be searched
+fromIndex - the index of the first element</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (inclusive)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to be searched
+toIndex - the index of the last element</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (exclusive)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to be searched
+key - the value to be searched for
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Returns:
+index of the search key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, if it is contained in the array within the specified range; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>otherwise, (-(insertion point) - 1).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The insertion point is defined as the point at which the key would be inserted into the array: the index of the first element in the range greater than the key, or toIndex if all elements in the range are less than the specified key. Note that this guarantees that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>return value will be &gt;= 0 if and only if the key is found.</t>
+    </r>
+  </si>
+  <si>
+    <t>LinkedIn 
+Google 
+Bloomberg 
+Facebook</t>
+  </si>
+  <si>
+    <t>Count Numbers with Unique Digits</t>
+  </si>
+  <si>
+    <t>Pow(x, n)</t>
+  </si>
+  <si>
+    <t>Implement Pow(x, n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Anagram </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corner cases:
+1. "bb" and "ac"
+2.  "aac" and "acc" </t>
+  </si>
+  <si>
+    <t>Given two strings s and t, write a function to determine if t is an anagram of s.
+For example,
+s = "anagram", t = "nagaram", return true.
+s = "rat", t = "car", return false. 
+Note:
+You may assume the string contains only lowercase alphabets.
+Follow up:
+What if the inputs contain unicode characters? How would you adapt your solution to such case?</t>
+  </si>
+  <si>
+    <t>Amazon 
+Uber 
+Yelp</t>
+  </si>
+  <si>
+    <t>Find All Anagrams in a String</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sliding Window Solution----Substring problem template!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Corner cases:
+1. the larger string is ""
+2. the larger string is shorter than the other string</t>
+    </r>
+  </si>
+  <si>
+    <t>Given a string s and a non-empty string p, find all the start indices of p's anagrams in s.
+Strings consists of lowercase English letters only and the length of both strings s and p will not be larger than 20,100.
+The order of output does not matter.
+Example : 
+Input:
+s: "abab" p: "ab"
+Output:
+[0, 1, 2]
+Explanation:
+The substring with start index = 0 is "ab", is anagram
+The substring with start index = 1 is "ba"
+The substring with start index = 2 is "ab"</t>
   </si>
 </sst>
 </file>
@@ -1880,7 +2292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1898,9 +2310,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1909,9 +2318,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1928,8 +2334,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2409,201 +2824,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>103185</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>435181</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1166865</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>513181</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="64" name="Ink 63">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09DF1DE7-C262-424E-BC49-2AA81A01E965}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="6383040" y="789600"/>
-            <a:ext cx="1063680" cy="78000"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="64" name="Ink 63">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09DF1DE7-C262-424E-BC49-2AA81A01E965}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6378720" y="785287"/>
-              <a:ext cx="1072319" cy="86627"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>121665</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>150468</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1290705</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>37155</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="66" name="Ink 65">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74304B55-1E9E-4E0B-9F85-E819349873B5}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="6401520" y="1424160"/>
-            <a:ext cx="1169040" cy="71280"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="66" name="Ink 65">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74304B55-1E9E-4E0B-9F85-E819349873B5}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6397200" y="1419840"/>
-              <a:ext cx="1177681" cy="79920"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>29505</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>427981</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1141905</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>504301</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="68" name="Ink 67">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30C145DD-85C5-4E9D-B11F-E4738B503F45}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="6309360" y="782400"/>
-            <a:ext cx="1112400" cy="76320"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="68" name="Ink 67">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30C145DD-85C5-4E9D-B11F-E4738B503F45}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6305040" y="778080"/>
-              <a:ext cx="1121040" cy="84960"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
       <xdr:colOff>826364</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>689184</xdr:rowOff>
@@ -2616,7 +2836,7 @@
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="72" name="Ink 71">
               <a:extLst>
@@ -2974,6 +3194,266 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>421084</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>284538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2806804</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>613578</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C630F8B-E974-4980-A66C-A755E8295D76}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6699840" y="150649440"/>
+            <a:ext cx="2385720" cy="329040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C630F8B-E974-4980-A66C-A755E8295D76}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6695520" y="150645120"/>
+              <a:ext cx="2394360" cy="337680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>71164</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>99018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4064284</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>1474938</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="13" name="Ink 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F63D4B16-5F79-4864-A26F-B7DEA7D3693D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6349920" y="150463920"/>
+            <a:ext cx="3993120" cy="1375920"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="13" name="Ink 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F63D4B16-5F79-4864-A26F-B7DEA7D3693D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6345600" y="150459600"/>
+              <a:ext cx="4001760" cy="1384560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2143324</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>1254378</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2143564</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>1254618</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="50" name="Ink 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17BD7344-3C21-4254-AA02-CD937D29B8C1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8422080" y="151619280"/>
+            <a:ext cx="240" cy="240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="50" name="Ink 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17BD7344-3C21-4254-AA02-CD937D29B8C1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8419200" y="151616400"/>
+              <a:ext cx="6000" cy="6000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2025604</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>613098</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2856124</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>1298178</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="71" name="Ink 70">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DBD39E4-7950-4B0F-BDFF-EFF6410A86D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8304360" y="150978000"/>
+            <a:ext cx="830520" cy="685080"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="71" name="Ink 70">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DBD39E4-7950-4B0F-BDFF-EFF6410A86D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8300040" y="150973680"/>
+              <a:ext cx="839160" cy="693720"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3483,114 +3963,6 @@
           <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2016-10-27T15:20:35.166"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
-      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
-      <inkml:brushProperty name="color" value="#ED1C24"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:traceGroup>
-    <inkml:annotationXML>
-      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
-        <emma:interpretation id="{262E3338-2AB5-4325-B9C2-82267B6A81A1}" emma:medium="tactile" emma:mode="ink">
-          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="17525,2361 20612,2144 20616,2193 17528,2409" shapeName="None"/>
-        </emma:interpretation>
-      </emma:emma>
-    </inkml:annotationXML>
-    <inkml:trace contextRef="#ctx0" brushRef="#br0">8763 1282,'0'0,"0"0,0 0,0 0,0 0,16 2,19 2,19 1,18-1,18-3,14-3,8-4,8-6,0-2,1-2,-2 0,-3 1,-3 1,-3 1,-3 2,-3 2,-6 1,-6 2,-6 2,-5 1,-4 2,-6-1,-5 0,-5-2,-4 0,-1 1,-1 1,-2 0,-2 1,0-1,-2 0,-3 0,0-2,-1 1,0 0,-1 1,-2-1,-2 0,1 1,-2 0,-3-2,-4 2,-3-1,-6 2,-4-1,-4 2,-3-1,-1 1,-4 0</inkml:trace>
-  </inkml:traceGroup>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2016-10-27T15:21:12.397"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
-      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
-      <inkml:brushProperty name="color" value="#ED1C24"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:traceGroup>
-    <inkml:annotationXML>
-      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
-        <emma:interpretation id="{9A41DFCB-8B42-4D62-9EB1-AA8BA200BCCE}" emma:medium="tactile" emma:mode="ink">
-          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="19736,203850 23309,203670 23312,203741 19739,203920" shapeName="None"/>
-        </emma:interpretation>
-      </emma:emma>
-    </inkml:annotationXML>
-    <inkml:trace contextRef="#ctx0" brushRef="#br0">9870 102010,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,15 0,6 0,-1 0,11 0,1 0,16 3,14 0,13 1,9-2,3 0,3 0,6-2,2 0,4 0,-2 0,4-2,2-2,4 0,-1-1,-7 0,-7-2,1 0,-1-1,-1 1,-6 1,-5 2,-6-1,-4-2,-3 0,-1 1,-5-1,-4 1,-6 1,-4 2,-6 1,-4 1,-2 0,4 2,4-1,2 0,2 1,-2-4,0 0,0-1,-2 0,-2-2,-4-1,-1 0,-2 2,1 1,0 2,4-2,-2 0,-2-2,-2 0,-5 1,-5 2,-5 0,-2 3,-6-1,-3 1,-6 0</inkml:trace>
-  </inkml:traceGroup>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2016-10-27T15:21:17.869"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
-      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
-      <inkml:brushProperty name="color" value="#ED1C24"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:traceGroup>
-    <inkml:annotationXML>
-      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
-        <emma:interpretation id="{6A944570-4C92-4BB0-9E06-1D594CBFC2DA}" emma:medium="tactile" emma:mode="ink">
-          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="19648,205570 23842,205122 23858,205263 19663,205710" shapeName="None"/>
-        </emma:interpretation>
-      </emma:emma>
-    </inkml:annotationXML>
-    <inkml:trace contextRef="#ctx0" brushRef="#br0">9832 103045,'0'0,"21"0,6 0,0 0,-7 0,-4 0,-7 0,16-4,15-4,11 2,9-2,10 1,4-1,-1-2,1 1,0 1,0 1,4 0,-2 0,3-2,2 0,4 0,5-4,3-3,1-4,0 0,-3-3,1 1,3-2,4 1,-3 2,-4 1,0 5,2 1,2 5,-1 2,-6 4,-3 1,0 1,1 2,0 0,2-1,1 1,-2-1,3 1,0-1,-2 0,-3-3,-2-3,-7-1,-3 1,-3 2,-4-2,-3 1,-7 1,-5 1,-10 1,-6 1,-9 1,-7 0,-7 0,-5 0</inkml:trace>
-  </inkml:traceGroup>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
       <inkml:timestamp xml:id="ts0" timeString="2016-10-27T15:22:29.337"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
@@ -3613,7 +3985,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -3686,7 +4058,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -3810,6 +4182,451 @@
           <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2317">14756 28038,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-17 2,-5 2,2-1,2 0,7-2,-13 0,-2 0,4-1,5 0,-5 0,1 0,5 0,3 0,-5 5,0 1,3 0,-5 1,1-4,5 0,-1 3,2 1,3-1,-5 4,-1 4,-1 0,-2 1,3 4,1 2,1 1,2 0,1 0,2 0,0-2,-2-1,2 0,3 0,0 0,3-1,2-2,1 1,0 0,6 7,4 5,7 8,1-2,6 1,5 0,6-3,6-4,1-4,-1-7,1-3,-3-7,-3-4,0-2,-2-2,0 0,2-4,3-6,6-4,4-3,1-3,0-3,-2 1,-5-1,-3 2,-2-3,-3 0,-2-3,-8-1,-4-5,-4-6,-1-5,-4 0,-5 4,-1 2,-4 2,-2 6,-2 2,-5 3,-2 5,1 0,-2 1,-2 5,-3-2,-4 0,-2 5,-3 2,1 2,-2 1,-1 3,-3 1,-1 1,-2 1,3 1,1-1,1 0,1 2,2-2,1 0,2 0,1 0,3 0,2 0,0 3,0 0,0 0,0 2,-1 3,1-1,-2 2,2-1,-1 2,-1 0,4-1,0 0,4-1,-2 2,4-3</inkml:trace>
           <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16267">12172 30979,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-18 0,-7 0,1 0,4 0,-13 0,-2 0,-4 2,3 2,-2 1,4 1,-2 7,-1 6,4 5,0 6,5 3,4 1,3 0,6 0,1-5,5-1,2-3,4 0,2-3,0 1,2-2,-1 2,1-2,0 1,-1 1,0-1,0 3,4 1,-1 5,6 1,4 3,4 4,7 3,4-1,6-2,5-4,2-3,5-3,-3-5,2-6,0-4,-1-7,-1-3,1-4,2 0,2-1,3-3,3 0,-3-3,-1-2,-1-3,-4 0,-4-5,-2-5,-3-4,-4-8,0-2,-2 1,-6-3,-3 3,-4 2,-4 3,-3 0,-2 1,0-1,-3-2,-2-1,-1 0,-2 0,0 3,0-2,0 4,-1 1,1 0,-4 2,-2 0,-4 3,-2 1,-3 2,0 3,-2-1,1 2,-4 1,-1-1,-2 1,2-1,-4 3,2-3,-4 3,3 3,0-1,0 4,0-1,0 4,3 2,1 0,-2 1,1 0,2 1,0-1,2 0,-1 0,2 1,-1-1,4 0,1 0,3 0,2 0,0 0,0 0,-2 0</inkml:trace>
           <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="94122">11466 28558,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,16-4,6-2,-1 1,13-6,-1-1,-5 1,-7 3,-8 4,4 0,-1 3,-3 1,-6 0,-1 1,-3-1,-2 0,-1 1,-1-1,0 0,1 0,0 0,-1 0,1 0,4 7,2 1,0 1,-4 9,-2 0,-2 7,-2-5,-3 0,-1-1,-1-4,-1 0,2-5,2-2,3 2,-1-3,4-2,-1 0,2-3,-1-2,0 0,0 0,1 0,-1 0,0-1,0 1,0 0,0-1,3 1,2 0,4 0,6-2,9-3,1-1,1-1,5 0,-2 2,-4-1,-2 1,-6 1,-6 0,-3-2,-2 3,0 0,-1 2,-1 0,1 1,-1 0,-1 0,-1 0,3 0,-2 1,1-1,-1 0,-2 0,0 0,-1 0,2-2,3-2,1 2,0 0,-2 0,1 1,-1 1,0-1,-1 1,-2 0,0 1,-1-1,0 0,0 0</inkml:trace>
+        </inkml:traceGroup>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2016-12-22T02:30:33.929"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{CEFFC407-DFB5-4945-8934-60BCF5748CF9}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="18611,418390 25246,418471 25234,419472 18599,419392" semanticType="scratchOut" shapeName="Other">
+            <msink:sourceLink direction="with" ref="{580BA9EB-EFCB-460A-A696-8C4E87AD9940}"/>
+            <msink:sourceLink direction="with" ref="{758E366B-9549-4592-A820-631B8C20F1CC}"/>
+            <msink:sourceLink direction="with" ref="{C9D5966F-2E96-4E1E-854F-C19405131228}"/>
+            <msink:sourceLink direction="with" ref="{78FB9D78-1799-4D80-B1EF-B0DF04DC2956}"/>
+            <msink:sourceLink direction="with" ref="{BA4B0AF8-6392-4282-903A-44672EB00C12}"/>
+            <msink:sourceLink direction="with" ref="{60213CF2-6932-4039-81E5-DD1BCCBB17EB}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">9307 209264,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,10 1,11 1,7-2,9 0,4-1,5 0,4-1,3-1,2 1,1 0,2 2,2-1,-2 0,-2 1,-3 0,-2 0,-3 0,-2 0,-2 1,-2 0,-2 1,-2 0,-4 1,0 0,-2 1,1 0,0-1,0-1,1-1,-2 1,-4 1,0-2,-2 1,1-1,2 0,-1-1,0 0,-2 0,0 0,-2 0,2 0,-1 0,2-1,2 1,0 0,3 0,0 0,2 0,0 0,0 0,0 0,0 0,0 0,0 0,2 0,0 0,2 0,1 0,4 0,0 0,3 0,2 0,2 0,1 0,0 0,1 0,0 0,1 0,3 0,0 1,-2 1,1 0,0 0,2-1,2 0,2-1,1 0,3 2,-1 0,1-1,-2 1,-1-1,1-1,-1 0,-2 1,0-1,0 0,4 0,0 0,4 0,2-1,1 1,1 0,1 0,1 0,-1 0,2 0,1 0,2 0,2-1,-2-1,-2 0,-4-1,-2 0,-3 0,-3 2,-1 0,-4 0,-1 0,-1 1,-3 1,1-1,0 0,-2-1,1-1,-4 0,0-1,2 0,-2 1,-1 0,-2 0,0 2,-1-2,-1 0,0 0,-1 1,-1 0,1-1,0 0,-1 0,-4-1,-3-2,-4 1,-4 0,-5 2,-4 0,-3 1,-4 1,-2 0,-4 0,0 0,-1 0,-1 1,0-1,-2 0,0 0,-1 0,-1 0,0 0,0 0,2 0,-1 0,1 1,1 2,-1 1,1 1,-1 0,-1 1,0 4,0 3,3 5,0 3,-1 4,1 2,-1 0,0-1,-1 2,-1 1,0 4,0 4,1 3,2 1,-1-1,0-2,-1-4,-1-1,1 0,1 0,-1 0,-1-2,0-1,-1-3,0-4,0-5,0 0,0-3,0-3,0-1,0-3,0-2,0 0,0-3,0-2,0 2,0-1,0-1</inkml:trace>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2079">9436 210098,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,11 0,2 0,9-2,9 0,8-1,4 0,5 0,0 1,4 1,2-1,2 2,1 0,0 0,2-1,2-1,1 1,2-1,-1 1,-5 0,-2 1,-1 0,-1 0,2 0,2 0,1 0,4 0,2 0,2 0,1 0,1 0,0 0,1 0,-2 0,-1 0,-2 0,-1 0,1 0,-2 0,1 0,1 0,2 0,3 0,3 0,4 0,4 0,0 0,0 0,-4 0,-1 0,0-1,-2-1,-2 0,1 1,-1 0,-1-1,0-2,-2 0,-1 0,-2 2,-3 0,-1 2,0-1,1 1,-2 0,0 0,-1 0,-2 1,0-1,-2 1,2 1,0 0,0-1,0 1,-2-2,0 0,-3 0,-2 0,-1 0,-2 0,-3 0,-2 0,-2 2,-1 0,-1 0,1-1,-2 0,-2 0,0-1,-2 0,-4 0,1 0,0 0,1 0,-2 0,2 0,-2 0,2 0,2 0,-1 0,1 0,1 0,-1 0,-1 0,2 0,1 0,4 0,2 0,4 0,4 0,2 0,0 0,-2 0,2 0,-3 0,-4 0,-5 0,-6 0,-6 0,-4 0,-2 0,-3 0,-2 0,-3 0,-1 0,-4 0,-1 0,-2 0,0 0,-3 0,0 0,-3 0</inkml:trace>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="547">9770 210150,'0'0,"0"0,0 0,0 0,-13 0,-5 0,2 0</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2016-12-22T02:30:45.572"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{5C711B6F-B9C4-4244-862E-72F30EFE695B}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="writingRegion" rotatedBoundingBox="17638,417955 28729,417955 28729,421776 17638,421776"/>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{1F5CDFFE-6E8B-444D-8D78-2A5771B16C60}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="18032,417933 28735,417994 28721,420373 18018,420312" alignmentLevel="1"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{453890F3-CE72-4CFC-8B96-162202A6BEB9}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkBullet" rotatedBoundingBox="18028,418649 18421,418651 18419,419025 18025,419022"/>
+            </emma:interpretation>
+            <emma:one-of disjunction-type="recognition" id="oneOf0">
+              <emma:interpretation id="interp0" emma:lang="zh-CN" emma:confidence="0">
+                <emma:literal>•</emma:literal>
+              </emma:interpretation>
+            </emma:one-of>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:trace contextRef="#ctx0" brushRef="#br0">8709 209512,'0'-1,"0"1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-6-9,-2-2,1 0,-8-5,-1-1,-4 1,-1 3,-2 0,1 3,-1 3,2 2,0 3,2 1,1 1,4 1,3-1,2 1,2-1,0 2,1 1,2 1,2 1,0 1,2 1,0 3,0 1,3 3,4 0,4 0,3 0,1 0,4 1,2 1,2 0,2 1,1-2,-2 0,-2-2,-3-1,-3-1,-3-1,-1-2,-4 0,-1-3,-2 0,-2-2,-2 1,0-1,-1 1,0 0,-2 1,-3 1,-3 0,-2 2,-4 0,-4-1,-4 0,-4-1,-4-1,-3-1,-1-1,1-1,5 0,2-2,5 0,4 0,5 0,1 0,2-1,3 1,0 0,0 0,1 0,2 0,0 0</inkml:trace>
+      </inkml:traceGroup>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{A79DE073-1014-46D8-8180-38851C082B1B}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="line" rotatedBoundingBox="18613,417936 28735,417994 28721,420373 18599,420315"/>
+            </emma:interpretation>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{758E366B-9549-4592-A820-631B8C20F1CC}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="18610,418472 18744,418472 18739,419333 18605,419332">
+                  <msink:destinationLink direction="with" ref="{CEFFC407-DFB5-4945-8934-60BCF5748CF9}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-13988">8898 209202,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 10,3 11,1 8,0-2,0 6,0 0,-1 3,0-3,1 3,0 3,1-2,-2 0,1-3,1-1,0 0,-1 0,1-2,1 1,-1-2,-2 2,1-3,-1-2,0-1,0-2,0-2,0-3,-1-2,-1-3,-1-2,0-2,-1-3,0 0,0-3,0 1,0-2,0 0,-1-1,1-1,0-1,0 0,0 0</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{C9D5966F-2E96-4E1E-854F-C19405131228}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="19427,418541 19531,418541 19527,419274 19422,419273">
+                  <msink:destinationLink direction="with" ref="{CEFFC407-DFB5-4945-8934-60BCF5748CF9}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-8088">9715 209271,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,3 13,1 5,0 12,-2 0,4 12,0 4,0 0,0 0,-1-4,0-2,1-4,-1-3,-1-1,0-3,0-1,-1-4,1 0,1-2,-1-1,0-2,-1-3,-1-2,-1-2,-1-2,0-2,0-2,0 1,-1-2,1 0,0 0,0-3,0 0,0 0,0-2,0 0,0 0,0 0,0 1,0 1,0 0,0 1,1-1,1 2,0 0</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{580BA9EB-EFCB-460A-A696-8C4E87AD9940}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="20385,417946 22227,417957 22213,420336 20371,420325">
+                  <msink:destinationLink direction="with" ref="{CEFFC407-DFB5-4945-8934-60BCF5748CF9}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24278">11032 208952,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,3 11,2 13,2 7,1 8,1 0,-1-2,-2-4,-2-6,-2-5,-1-4,0-5,-2-2,1-2,-1-3,1-1,0-2,0-3,0-1,0-2,4-3,5-6,3-5,3-6,2-3,0-1,2 0,-1 3,-2 3,0 3,-2 2,-1 4,-3 0,-2 5,-2 0,-2 2,0 2</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24772">11342 208883,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,13 13,5 5,-1-1</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24532">11462 209064,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,1 11,1 2,0 0,2 7,1-1,-1-3,0-5,-2-4</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25938">11815 209003,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-10 2,-4 0,2 0,-5 9,2 4,0 7,2 1,5 4,3 3,1-4,3-4,1-5,0-6,3-1,-1-4,3-1,2-4,3-6,3-7,1-9,1-5,-2-6,-2-2,-2 1,-2 3,-3 5,-1 8,-3 6,0 5,0 3,0 3,0 4,-1 7,0 11,1 8,0 7,0 10,0 9,0 4,0-3,0-5,-1-5,-2-6,-3-4,-2-2,-3-2,-4-4,-5-4,2-3,-1-5,1-7,1-3,2-4,2-3,2 0,2-4,0-4,3-2,3-5,6-9,5-9,9-9,6-10,9-6,5-8,3-6,-5 10</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26462">12125 208685,'0'0,"0"0,0 0,0 0,0 0,-1 9,-1 2,-5 18,-2 12,-2 12,-2 10,0 2,-1-4,2-5,0-6,2-9,2-9,2-12,3-7,2-7,0-5,1-1,2-2,3-4,3-6,2-6,2-4,1-2,0-1,-2 4,-2 4,-2 6,-2 4,-1 6,-1 3,1 7,-1 6,0 4,0 4,0-1,1-2,-1-4,2-4,-1-4,-2-4</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26860">12339 208848,'0'0,"0"0,0 0,0 0,-2 9,-2 2,-2 14,2 8,-3 8,0 2,1 1,2-1,2-7,1-7,0-6,1-4,3-6,3-4,2-2,5-4,-2-1</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27165">12159 209012,'0'0,"0"0,0 0,0 0,0 0,0 0,15-1,15-2,15-4,12-4,6-1,3-5,-10 1</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7263">10670 209305,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 11,0 5,0 9,1 8,1 7,2 6,0 4,3 4,-1 0,0 1,0-1,-1-4,0-4,-1-4,1-5,-2-4,-1-5,-1-5,-1-2,2-5,0 0,0-3,-1 0,0-3,-1-1,0 0,0-2,0 0,0-3,0-1,0-2</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22662">11600 210294,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,-2 10,-2 4,-4 6,-1 1,-2 3,1-3,0 4,1-4,0 0,2-4,3-2,1-4</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-6395">11626 209288,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 9,1 3,0 7,0 2,-1 5,0-1,-1 6,0 3,0 2,2 2,0-2,0-1,1-2,1-2,-2-4,-1-1,0-5,-1-2,0-2,0 0,0-1,0 1,0 0,0 0,0-2,0-3,0-2,0 0,0-1,0-4,0 1,0-2,0 1,0-2,0-1,0 0,0-2,0 2,0 0,0 0,0-2,0 2,0-2,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22233">11677 210191,'0'0,"0"0,0 0,0 0,0 0,4 9,2 3,-1-2,0 8,-2 8,1 7,0 8,0 3,0 0,-2-1,0-1,-2-2,0 1,2 0,0-1,0-3,-1-2,0-2,-1-2,2 0,2 1,0-1,-2 0,1-3,-1-2,-1-4,-1-4,0-4,0-5,0-3,0-3</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22979">11729 210182,'0'0,"0"0,0 0,0 0,0 0,10 6,4 2,6 7,1 0,1 3,-2-2,1 1,-3-3,-4-4,-6-3,2-1,-2-3</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-5474">12511 209219,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 11,0 5,0 9,0 1,0 7,0 3,0 2,-1 1,-1 0,1 3,-1-3,1-1,1-4,-1-4,1-4,0-2,0-3,0-3,0-3,0-2,1-4,-1 1,0-2,0 0,0 0,0-1,0-1,0-1,0-1,0 0,0 0,0 0,0 1,0-1,0-1,0-2,0 0,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{78FB9D78-1799-4D80-B1EF-B0DF04DC2956}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="23041,418480 23060,418480 23056,419250 23036,419249">
+                  <msink:destinationLink direction="with" ref="{CEFFC407-DFB5-4945-8934-60BCF5748CF9}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-4522">13329 209210,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 9,0 2,0 10,0 2,0 6,0 1,0-4,0 2,0-2,0-1,0-2,0 1,0-1,0 1,0 1,0-2,0 0,0 0,0-4,0-2,0-1,0-2,0 0,0 0,0-1,0 0,0-1,0-2,0 0,0 1,0 0,0 0,0 1,0 1,0-1,0 2,0 0,0 0,0-2,0 0,0-4,0-1,0-2,0 0,0 0,0-1,0 0,0-1,0 1,0 0,1 1,3-1,1 1,0-2</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{BA4B0AF8-6392-4282-903A-44672EB00C12}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="23738,418489 23768,418489 23764,419247 23733,419247">
+                  <msink:destinationLink direction="with" ref="{CEFFC407-DFB5-4945-8934-60BCF5748CF9}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-3763">14026 209219,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 10,0 4,0 9,0 9,0 4,0 2,0 0,0 1,0 1,0-2,0-3,0-1,0-3,1-3,1-2,0-2,0-2,0-1,1-3,-1 1,1-2,0-1,-1 2,0-2,-1 0,0 0,-1-2,0-1,0-2,0-1,0-2,0 0,0-3,0-1,0 0,0 1,0-1,0 0,0 0</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{60213CF2-6932-4039-81E5-DD1BCCBB17EB}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="24409,418532 24499,418532 24494,419316 24404,419315">
+                  <msink:destinationLink direction="with" ref="{CEFFC407-DFB5-4945-8934-60BCF5748CF9}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2827">14697 209262,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 12,1 3,0 9,0 0,0 6,1 5,0 2,1 3,0 2,2-2,-1-4,-1-4,-1-4,0-2,0-3,1 0,1-2,-1-1,0 0,-1 0,0 1,0 1,-1-2,0 1,-1-3,-1 0,2-5,0 0,0-2,-1-2,0-1,-1 2,0-3,0 0,0-1,0-2,0 1,0 0,0-1,0 0,0 0,0-2,0 0,0 0,0-2,0 0</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{006FAC3A-4929-4D33-B816-B71DA32D6C09}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="26070,418221 26460,418223 26456,418998 26065,418996"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4644">16358 208977,'9'-2,"2"-2,0 0,-1 1,-4 1,6-1,2 1,4-1,-1 2,6 0,7 2,2 2,3 2,-1 2,-2 2,-4 3,-4 4,-6 4,-4 2,-6 0,-4 3,-4 2,-4 2,-7 3,-4 4,-3 0,0-3,0-5,3-5,3-7,3-7,2-4</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4977">16642 209038,'0'0,"-2"13,1 5,-1-2,0-2,1 6,-1 11,0 11,-2 10,1 3,-2 3,1-2,-1-3,1-4,1-6,1-5,1-6,0-8,1-6,0-2,0-2,0-2,1-3,-1-2</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{96CAC439-0295-4E37-B45C-441468D5A4DA}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="26741,418507 28732,418519 28728,419181 26737,419169"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8959">17029 209287,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,13 2,5 0,12 0,10-1,6 0,7-1,4-2,-1 0,2-1,2 0,2-1,1-2,0 2,-1-2,-2 1,0 2,-3 0,-3 2,-2 0,-2 1,0 0,-2 0,-1 0,-1 1,1-1,-1 0,0 0,2 0,0 2,-2-1,2 1,-3-1,-2 1,-3-2,-1 2,-3 2,-2 0,-3-1,-5-1,-5 0,-4-1,-3-1,-3 0,-2 0,-3 0,-1 0,0 0,0 0,-2 0,-1 0,0 0,-2 0,0 0,2 0,0 1,-1 1,0 1,0 1,0 0,1 2,1 2,1 4,-1 4,1 2,0 2,0 2,2 3,-2 0,0 0,-1 2,0 1,0-2,-1-1,0 0,-1-3,-1-2,0-4,0 0,0-3,0-1,0 0,0-1,0-1,0 0,0 0,0-2,0 0,0-2,0 1,0-2,0-1,0 0,0 0,0 0,0 1,0 0,0-2,0 2,0-2,0 0,0 0,0 2,0-1,0-1,0 0,0-2,0 0,0-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0-1,0 3,0 0,0 1,0 2,0 0,-2-1,0-1,0-1,-1-1,-1-1,-2 2,0 0,-1-1,-2 0,0 1,-2-2,0 0,-1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,0 0,0 0,-1 0,0 0,-2 0,0 0,1 0,-2 0,0 0,0 0,0 0,0 0,-2 0,0 0,0 0,1 0,0 0,0 0,0 0,-1 0,0 0,-1 0,1 0,1 0,0 0,1 0,1 0,-1 0,2 0,2 0,0 0,0 0,2 0,-2 0,0 0,0 0,-1 0,1 0,-3 0,1 0,0 0,1 0,0 0,1 0,1 0,0 0,0 0,1 0,2 0,0 0,0 0,-1 0,0 0,2 0,-1 0,-1 0,-2 0,0 0,-1 0,-1 0,0 0,1 0,0 0,1 0,0 0,-1 0,2 0,0 0,0 0,0 0,2 0,-1 0,2 0,-1 0,2 0,-1 0,1 0,-1 0,-1 0,2 0,-1 0,-1 0,2 0,-1 0,0 0,1 0,0 0,-1 0,0 0,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,-2 0,2 0,0 0,-2 0,2 0,0 0,-2 0,0 0,2 0,-1 0,-1 0,2 0,-1 0,0 0,1 0,1 0,0 0,-1 0,1 0,-1 0,-1 0,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1 0,0 0,4 0,-2 0,1 0,1 0,-1 0,1 0,-1 0,-1 0,1 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,1 0,-1 0,0 0,1 0,0 0,0 0,0 0,0 0,-1 0,1 0,1 0,1 0,0 0,2 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5766">17055 209296,'0'0,"0"0,0 0,0 0,0 0,0 0,0 7,0 3,1 11,3 11,0 10,-1 8,0 4,-1 0,-1-4,-1-6,0-7,0-4,0-6,0-2,0-1,0-4,0-3,0-4,0-1,0-3,0 0,0-3,0-2,0-1,0-2</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10327">17649 209262,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 11,0 2,0 7,0 1,0 5,0 6,0 2,0 2,0-1,0-3,0-2,0-4,0-3,0-4,0-3,0-1,0-2,0-1,0 0,0-1,0 0,0-2,0 0,0-1,0 1,0-1,0-1,0-1,0-2,0 0,0 0,0 0,0-2,0 1,0 0,0-1,0 0,0-1,0 0,0-1,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11530">18277 209245,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 12,0 3,0 11,0 5,1 3,1-1,0-1,0 0,-1 0,0-1,-1-2,0-3,2-2,-1-2,1-3,0-2,-1-3,0-2,0-3,1 0,0-1,-1 0,1 1,-2-1,0 1,0 1,0-2,0 0,0 0,0-1,0-2,0-1,0 0,0 0,0 1,0 0,0-1,0 0,0-1,0 2,0 1,0-1,0-2,0 0,0-2,0-1,0 2,0 0,0 0,0-1,0 0,0-1,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+        </inkml:traceGroup>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{712E1AC2-6241-48EA-B3B3-BE90B6D7F7E3}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="17638,419065 21389,419065 21389,420347 17638,420347" alignmentLevel="1"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{44347F03-AE4E-478B-9580-B2008407C04F}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="line" rotatedBoundingBox="17638,419065 21389,419065 21389,420347 17638,420347"/>
+            </emma:interpretation>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{F8C40BFA-B055-498A-BF39-6727019837AD}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="17638,419065 18888,419065 18888,420193 17638,420193"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15949">8993 210269,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-3 11,0 2,-1 0,-4 5,0-1,2-3,-3 3,2-1,0 1,1-3,2-2,1-6</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15428">9027 210234,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 13,0 10,2 9,-1 6,3 4,1 4,-1 2,2 2,-1 2,-2-2,0-2,-2-3,0-4,-1-5,0-5,0-6,0-6,0-5,-1-3,1-3,0-3,0-1,0-2,0 1,0-1,0-1,0-1,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16261">9036 210260,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,11 9,2 3,0-1,5 4,-1-1,-3-3,-4-3,3 2,0-2,-2-1,-4-3</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19285">8461 209795,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-8 11,-2 2,1 12,1 9,3 9,3 7,4 7,1 3,1 2,2 3,-1 1,1 0,0-4,-2-5,0-4,-2-1,-2-2,-1-3,-1-4,0-6,0-6,1-6,0-8,0-5</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19661">8605 210019,'0'0,"0"0,0 0,0 0,0 0,0 0,0 15,0 4,3 10,2 8,2 4,1 3,3-2,0-1,1-1,2-3,0-1,-1-3,-1-7,-3-8</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20039">8330 210320,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,10-1,4-1,11-3,11-2,8-2,6-2,4-2,1 0,3 0,0 0,-4 2,-3 1,-10 1</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18761">7960 209960,'0'0,"0"-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 13,-1 5,-2 15,0 9,-3 5,1 1,1-4,2-1,1-3,2-3,3-1,3-3,2-2,2-2,2-4,2-4,2-4,0-4,1-3,0-4,1-4,1-4,2-3,2-6,1-5,-1-4,0-3,-3-2,-3-3,-4 0,-4-3,-4 4,-2 3,-2 4,-1 4,0 3,-3 5,0 0,1 4,0 1,1 2,-1 0,-2 2,-1 2,-2 2,-1 2,1 4,1 4,0 2,2-1,1 0,2 1,0-1,1 1,3 0,5 0,2 0,6-1,1-4,2-3,2-4,3-5,3-4,-3-2</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{02EE219C-F606-4EF0-9034-D9EB559455FD}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="18948,419804 21390,419829 21385,420360 18942,420335"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31269">9250 210535,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 11,-1 2,0 0,-1 7,0-2,0 7,2-2,1 2,1 3,4-2,2 0,2-1,4-2,1-2,2-5,2-2,0-4,4-4,2-3,4-3,4-3,3-2,5-2,5-3,2-4,0-4,-1 2,-4-1,-1 2,0 0,0 1,-2 4,-4 2,-4 4,-3 1,-2 2,-2 1,0 2,1 4,3 5,1 4,-1 5,-1-1,-3 2,-1 1,-3 0,-3-1,-4 0,-1 2,-3 1,0 0,-3-2,-1-3,-2-1,-2-4,0-4,-1-2,-1-2,0-2,1-1,0-2,1-2,2-2,3-5,2-5,3-2,2-4,0 0,0 0,1 1,3 1,2 2,2 0,3 1,1 1,0 1,0 3,0 2,-1 2,2 2,3 2,2 1,1 0,3 1,1 0,2 2,0-1,1 1,1 0,-4 0,0-1,-1-1,-2-1,-1 1,0-1,-2 0,0-1,0 1,-2 0,2-1,0-3,1-3,0-1,-1-3,0-2,-4-3,-3 0,0 1,-4 0,-1 3,-5 1,0 3,-2 0,-3 2,-2 0,-1 2,0-1,-1 2,0 1,0 1,-2 0,1 1,-2 0,1 1,-2-1,0 0,0 1,0-1,0 0,0 0</inkml:trace>
+        </inkml:traceGroup>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{ECA666A4-375B-413D-BC0D-09829A5151F3}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="19741,420184 22389,420184 22389,420848 19741,420848" alignmentLevel="2"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{E36091C6-2F59-4700-B22C-D5D452AAA4C7}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkBullet" rotatedBoundingBox="19741,420184 22389,420184 22389,420848 19741,420848"/>
+            </emma:interpretation>
+            <emma:one-of disjunction-type="recognition" id="oneOf1">
+              <emma:interpretation id="interp1" emma:lang="zh-CN" emma:confidence="0">
+                <emma:literal>→</emma:literal>
+              </emma:interpretation>
+            </emma:one-of>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33801">10051 210914,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-4 11,-2 2,1 7,0 1,3 4,2-1,4 3,1 3,3 0,2 0,4 2,0-1,3-3,2-1,1-3,-1-2,2-5,1-6,2-4,0-3,4-3,3-4,7-3,3-2,3 0,0 0,-4 0,-2 1,-2 1,0-1,1 2,0-1,-1 2,-2 1,0 1,-1 0,-3 2,1 0,3 1,4 3,-1 1,0 2,-2 2,-1 5,-1 1,-3 0,-2 3,-4 0,-3-1,-2-2,-1 1,-2-3,0 1,-3-1,-2-1,-2 1,-2 0,0-1,0 2,-2-2,-1 0,-1-3,-1-1,-1-2,-1-3,0 0,-1-2,1-1,-1 0,1 0,0-1,0-1,2-1,1-5,2-4,3 0,4-5,2 0,1 1,2-2,1 1,0 3,4 1,2 1,2 2,2 0,0 3,3 0,0 1,-1 2,0 2,2 1,2 0,3 1,-1 1,-1-1,-2 1,1-1,-1 0,0 0,1 0,1 0,-1 0,-2-2,-2-1,0 0,0-3,0-1,1-2,-1-2,0-1,0-1,-3 0,-1 0,-2 0,-1-1,-2 2,-3-2,-3-2,0-2,-2-2,0 0,-2 0,-2-3,-1 2,0 2,-1 4,-2 3,-3 2,0 2,-2 2,0 2,0 1,0 0,0 0,-1 1,1 1,0 0,0 1,0-1,0 2,0-1,0 0</inkml:trace>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{0DC23A7A-BA3E-41A6-973B-8EFC65FC9CF3}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="20718,420648 25288,420648 25288,421776 20718,421776" alignmentLevel="3"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{654EFA25-E0F8-43EA-B22B-D01CCEBA3888}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="line" rotatedBoundingBox="20718,420648 25288,420648 25288,421776 20718,421776"/>
+            </emma:interpretation>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{B3D7D31E-530C-458E-AD65-3B53B8EFB0C7}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="20718,420648 25288,420648 25288,421776 20718,421776"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38350">13811 211938,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40412">13562 211989,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,3 9,1 2,1 10,0 2,2 4,0-3,-1 1,0-4,3-2,0-3,4-1,4-1,4-1,3-3,3-2,4-3,2-1,1-2,0-1,-1 0,-2-2,-1 2,1 1,1-1,1 0,0 2,0 1,-1 3,0 0,0 2,-2 1,-2 2,-3 0,-2 1,0 1,-4 0,-1 1,-2-2,-1 1,-2-1,-3 0,-3 0,-2-1,1-2,-2-2,0 0,-2-3,-2 0,1-1,-1-1,0-1,-1-1,1-1,0 0,2 0,0 0,0-4,4-1,0-4,3-4,2-3,3-1,2-1,2 1,2 0,0 1,3 0,1 3,1 0,0 1,0 0,-1 2,-1 1,-1 0,2 2,-2 2,-1 1,0 3,1 0,2 1,-2 0,0 1,-2 0,-1-1,-1 0,-1 0,2 0,0 0,0 0,0 0,0 0,4 0,1 0,4-2,0-1,-1 0,-2-1,-4 0,-2-1,0 0,-2 0,-2-1,0-1,-1-1,0-2,0 0,-1-2,1 0,-1-2,1 2,0 0,-2 1,-2 1,0-1,0 0,-2 1,-1 0,0 1,-1-1,0 2,-2 0,-2 2,0 0,-2 3,0 1,0 1,0 0,0 1</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35874">11006 211482,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,3 9,1 3,0-2,-2 8,0 0,0 5,-2-2,2-1,0-2,2-1,-1-3,1 1,0-4,2 3,3-2,1-2,3 0,1 0,0-2,2-1,3-3,2-1,2-2,3 1,3 0,2-1,1 1,2-2,-1 0,1 0,1 0,1 0,0 0,0 0,2 0,0 2,2 0,0 1,0 0,0 3,2 2,-2 2,0 2,-4 3,-4 2,-2 2,-2 0,-2-1,-4-1,-2-2,-3-2,-3-2,-3-1,-1-1,-2-2,-2-1,0 1,-1-2,-1-1,-2-2,-1 0,0-2,-1 0,0 0,-1 0,1 0,0 0,1 0,1 0,3-2,5-3,3-5,3-4,4-3,1-1,3 0,1 0,1-1,1 3,2 1,-1 5,0 1,-1 3,0 1,0 1,1 0,1 0,3 2,2 0,0 1,-1 0,1 1,-1 0,3 0,0 1,2-2,0-1,0-2,0 0,-3-2,2-2,-3 0,-1-1,-1-1,-2-1,-1-3,-1-2,-2 0,-1-2,-3-1,-1-1,-6 0,-1 3,-2 0,-3 1,-1 0,-2 1,0 0,-1 2,-1 0,-1 0,1 0,0-3,0 1,0 2,-2 1,0 2,-2 2,0 1,0 3,0 0,0-1,0 1,0 1,0 1,0 1,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37932">13175 211972,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+        </inkml:traceGroup>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2016-12-22T02:31:23.720"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{DCC0EBBC-E916-4201-A1D7-06530A4DC202}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing"/>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">11699 210584,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2016-12-22T02:31:26.644"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{418FDC1D-50B2-469E-8813-B77645E2F879}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="writingRegion" rotatedBoundingBox="23007,419389 25373,419233 25502,421201 23137,421357"/>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{023D7A08-0E21-410B-A61A-8505CC4FEB85}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="23007,419389 25373,419233 25502,421201 23137,421357" alignmentLevel="1"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{9E72A7F1-FF97-42A0-8530-508206F3455B}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="line" rotatedBoundingBox="23007,419389 25373,419233 25502,421201 23137,421357"/>
+            </emma:interpretation>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{2BE23CE0-E513-4855-BA1A-8CB240B3CB38}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="23007,419389 23282,419371 23409,421299 23134,421317"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0">13398 210113,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="363">13355 210776,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 15,0 6</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="206">13381 210586,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="535">13434 211146,'-1'0,"1"0,2 9,0 3,-1-2,1-1,-1-3,-1-2</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="722">13476 211490,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="880">13553 211765,'0'0,"0"0,1 9,1 3,1-2,-2-1,0-3</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1051">13682 212015,'0'0,"0"0,0 0,0 0,0 0</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{4F17FD78-ED38-4660-B026-CAB630EB3874}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="25053,419482 25387,419460 25502,421201 25168,421223"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2234">15515 211214,'0'0,"0"0,0 0,0 0,0 0,1 9,1 2,0 8,-1-1,1 8,-2-1</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1885">15609 210595,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2071">15635 210914,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2391">15489 211654,'0'0,"0"0,0 0,0 1,0-1,2 13,1 4,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2557">15455 211938,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3735">15506 211731,'0'0,"0"0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3625">15549 211396,'0'0,"0"0,0 0,0 0,0 0,0 18,0 5</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3135">15463 210216,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3444">15515 210888,'0'0,"0"0,1 12,1 3,0 1,-1-4,1-4,-2-3</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3265">15541 210552,'0'0,"0"0,0 0,0 0,0 0</inkml:trace>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1687">15661 210191,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0</inkml:trace>
         </inkml:traceGroup>
       </inkml:traceGroup>
     </inkml:traceGroup>
@@ -4322,7 +5139,7 @@
           <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2016-10-27T15:20:29.196"/>
+      <inkml:timestamp xml:id="ts0" timeString="2016-10-27T15:21:12.397"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.02333" units="cm"/>
@@ -4334,12 +5151,12 @@
   <inkml:traceGroup>
     <inkml:annotationXML>
       <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
-        <emma:interpretation id="{3FD4EBDB-4D46-4D3C-A0C1-FBD33FAD10CA}" emma:medium="tactile" emma:mode="ink">
-          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="17727,2347 20678,2126 20685,2211 17733,2432" shapeName="None"/>
+        <emma:interpretation id="{9A41DFCB-8B42-4D62-9EB1-AA8BA200BCCE}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="19736,203850 23309,203670 23312,203741 19739,203920" shapeName="None"/>
         </emma:interpretation>
       </emma:emma>
     </inkml:annotationXML>
-    <inkml:trace contextRef="#ctx0" brushRef="#br0">8867 1283,'0'0,"0"0,0 0,0 0,0 0,0 0,12 6,13 0,14 1,17 0,17-3,14-5,14-4,7-7,4-5,4-1,1-1,2 1,-3 0,0 1,-4 2,-4 2,-4 1,-8 1,-7 2,-11 2,-8 1,-9 0,-9 1,-5 2,-1 1,-2 1,-2 0,2 1,-2 0,-3 1,-3-1,-2 0,-3 0,-5 0,-2 0,0 0,0 0,-2 0,2 0,1 0,0 0,1 0,0 0,-2 0,2 0,0 0,0 0,-1 0,-2 0,-1 0,0 0,-1 0,-2 0,-3 0,-2 0,-2 0,-1 0,-2 0,-3 0,-1 0,-1 0,0 0,2 0,-1 0,-1 0,0 0,-2 0,-2 0</inkml:trace>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">9870 102010,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,15 0,6 0,-1 0,11 0,1 0,16 3,14 0,13 1,9-2,3 0,3 0,6-2,2 0,4 0,-2 0,4-2,2-2,4 0,-1-1,-7 0,-7-2,1 0,-1-1,-1 1,-6 1,-5 2,-6-1,-4-2,-3 0,-1 1,-5-1,-4 1,-6 1,-4 2,-6 1,-4 1,-2 0,4 2,4-1,2 0,2 1,-2-4,0 0,0-1,-2 0,-2-2,-4-1,-1 0,-2 2,1 1,0 2,4-2,-2 0,-2-2,-2 0,-5 1,-5 2,-5 0,-2 3,-6-1,-3 1,-6 0</inkml:trace>
   </inkml:traceGroup>
 </inkml:ink>
 </file>
@@ -4358,7 +5175,7 @@
           <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2016-10-27T15:20:32.413"/>
+      <inkml:timestamp xml:id="ts0" timeString="2016-10-27T15:21:17.869"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.02333" units="cm"/>
@@ -4370,12 +5187,12 @@
   <inkml:traceGroup>
     <inkml:annotationXML>
       <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
-        <emma:interpretation id="{E7FF7B9F-14FA-4B4F-A904-384AA8F95C64}" emma:medium="tactile" emma:mode="ink">
-          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="17780,4129 21023,3892 21028,3961 17785,4198" shapeName="None"/>
+        <emma:interpretation id="{6A944570-4C92-4BB0-9E06-1D594CBFC2DA}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="19648,205570 23842,205122 23858,205263 19663,205710" shapeName="None"/>
         </emma:interpretation>
       </emma:emma>
     </inkml:annotationXML>
-    <inkml:trace contextRef="#ctx0" brushRef="#br0">8892 2180,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,15 0,19 0,12 0,12 0,9 0,11 0,12 0,5-2,5 0,2-2,4-2,2-2,-1 1,2-2,2-4,-1-1,-1-1,-1-2,-4-1,-1 3,-2 0,-2 1,-3 1,-8 2,-5 3,-6 2,-4 3,-7 2,-5 0,-4 1,-2 1,-1-1,-4 1,-2-1,-2 1,-1-1,-1 0,-1 0,-3 0,-2 0,-1 0,-2 0,-3 0,-6 0,-4 0,-3 0,-2 0,-2 0,-4 0,-3 0</inkml:trace>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">9832 103045,'0'0,"21"0,6 0,0 0,-7 0,-4 0,-7 0,16-4,15-4,11 2,9-2,10 1,4-1,-1-2,1 1,0 1,0 1,4 0,-2 0,3-2,2 0,4 0,5-4,3-3,1-4,0 0,-3-3,1 1,3-2,4 1,-3 2,-4 1,0 5,2 1,2 5,-1 2,-6 4,-3 1,0 1,1 2,0 0,2-1,1 1,-2-1,3 1,0-1,-2 0,-3-3,-2-3,-7-1,-3 1,-3 2,-4-2,-3 1,-7 1,-5 1,-10 1,-6 1,-9 1,-7 0,-7 0,-5 0</inkml:trace>
   </inkml:traceGroup>
 </inkml:ink>
 </file>
@@ -4677,26 +5494,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG125"/>
+  <dimension ref="A1:AG135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="91" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E130" sqref="E130:E132"/>
+      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.54296875" customWidth="1"/>
     <col min="2" max="2" width="4.1796875" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" style="8" customWidth="1"/>
     <col min="4" max="4" width="56.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="60.36328125" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="5.36328125" customWidth="1"/>
-    <col min="10" max="31" width="10.90625" style="9" customWidth="1"/>
-    <col min="32" max="33" width="8.7265625" style="9"/>
+    <col min="5" max="5" width="60.36328125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="5.36328125" style="8" customWidth="1"/>
+    <col min="10" max="30" width="10.90625" style="8" customWidth="1"/>
+    <col min="31" max="31" width="19.54296875" style="8" customWidth="1"/>
+    <col min="32" max="33" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4712,7 +5530,7 @@
       <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -4721,10 +5539,10 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>282</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -4790,11 +5608,13 @@
       <c r="AD1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
+      <c r="AF1" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="AG1" s="7"/>
     </row>
     <row r="2" spans="1:33" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -4806,7 +5626,7 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
@@ -4856,7 +5676,7 @@
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -4899,7 +5719,7 @@
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4944,7 +5764,7 @@
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -4989,7 +5809,7 @@
       <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
@@ -5034,7 +5854,7 @@
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
@@ -5083,7 +5903,7 @@
       <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="13" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -5133,7 +5953,7 @@
       <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="2" t="s">
         <v>32</v>
       </c>
@@ -5181,7 +6001,7 @@
       <c r="D10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="13" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -5231,7 +6051,7 @@
       <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="13" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -5282,7 +6102,7 @@
       <c r="C12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="2" t="s">
         <v>48</v>
       </c>
@@ -5321,7 +6141,7 @@
       <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -5371,7 +6191,7 @@
       <c r="D14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="13" t="s">
         <v>54</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -5421,7 +6241,7 @@
       <c r="D15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="13" t="s">
         <v>55</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -5471,7 +6291,7 @@
       <c r="D16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="13" t="s">
         <v>60</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -5516,7 +6336,7 @@
       <c r="C17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="13" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -5559,7 +6379,7 @@
       <c r="C18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="6"/>
       <c r="G18" s="2"/>
       <c r="J18" s="2"/>
@@ -5601,7 +6421,7 @@
       <c r="D19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="13" t="s">
         <v>67</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -5651,7 +6471,7 @@
       <c r="D20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="13" t="s">
         <v>86</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -5703,7 +6523,7 @@
       <c r="D21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="13" t="s">
         <v>83</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -5750,7 +6570,7 @@
       <c r="C22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="13" t="s">
         <v>76</v>
       </c>
       <c r="F22" s="2" t="s">
@@ -5798,7 +6618,7 @@
       <c r="D23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="2" t="s">
         <v>32</v>
       </c>
@@ -5844,7 +6664,7 @@
       <c r="D24" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="2" t="s">
         <v>81</v>
       </c>
@@ -5887,7 +6707,7 @@
       <c r="C25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="2" t="s">
         <v>84</v>
       </c>
@@ -5933,7 +6753,7 @@
       <c r="D26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="6"/>
       <c r="G26" s="2"/>
       <c r="J26" s="2"/>
@@ -5975,7 +6795,7 @@
       <c r="D27" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="13" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="2" t="s">
@@ -6027,7 +6847,7 @@
       <c r="D28" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="16" t="s">
         <v>101</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -6077,7 +6897,7 @@
       <c r="D29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="2" t="s">
         <v>100</v>
       </c>
@@ -6123,7 +6943,7 @@
       <c r="D30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="13"/>
       <c r="F30" s="2" t="s">
         <v>100</v>
       </c>
@@ -6169,7 +6989,7 @@
       <c r="D31" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="13" t="s">
         <v>108</v>
       </c>
       <c r="F31" s="2" t="s">
@@ -6219,7 +7039,7 @@
       <c r="D32" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="13" t="s">
         <v>104</v>
       </c>
       <c r="F32" s="2" t="s">
@@ -6269,7 +7089,7 @@
       <c r="D33" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="13"/>
       <c r="F33" s="2" t="s">
         <v>32</v>
       </c>
@@ -6315,7 +7135,7 @@
       <c r="D34" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="13" t="s">
         <v>112</v>
       </c>
       <c r="F34" s="2" t="s">
@@ -6365,7 +7185,7 @@
       <c r="D35" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="13" t="s">
         <v>115</v>
       </c>
       <c r="F35" s="2" t="s">
@@ -6414,7 +7234,7 @@
       <c r="C36" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="13" t="s">
         <v>120</v>
       </c>
       <c r="F36" s="2" t="s">
@@ -6458,7 +7278,7 @@
       <c r="D37" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F37" s="2" t="s">
@@ -6503,7 +7323,7 @@
       <c r="C38" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="13"/>
       <c r="F38" s="2" t="s">
         <v>32</v>
       </c>
@@ -6544,7 +7364,7 @@
       <c r="C39" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="13"/>
       <c r="F39" s="2" t="s">
         <v>32</v>
       </c>
@@ -6588,7 +7408,7 @@
       <c r="D40" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="13"/>
       <c r="F40" s="2" t="s">
         <v>128</v>
       </c>
@@ -6636,7 +7456,7 @@
       <c r="D41" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="13"/>
       <c r="F41" s="2" t="s">
         <v>81</v>
       </c>
@@ -6684,7 +7504,7 @@
       <c r="D42" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E42" s="6"/>
+      <c r="E42" s="13"/>
       <c r="F42" s="2" t="s">
         <v>81</v>
       </c>
@@ -6729,7 +7549,7 @@
       <c r="C43" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="13" t="s">
         <v>140</v>
       </c>
       <c r="F43" s="2" t="s">
@@ -6776,7 +7596,7 @@
       <c r="C44" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="13" t="s">
         <v>142</v>
       </c>
       <c r="F44" s="2" t="s">
@@ -6821,7 +7641,7 @@
       <c r="C45" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E45" s="6"/>
+      <c r="E45" s="13"/>
       <c r="F45" s="2" t="s">
         <v>69</v>
       </c>
@@ -6864,7 +7684,7 @@
       <c r="C46" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="13" t="s">
         <v>145</v>
       </c>
       <c r="F46" s="2" t="s">
@@ -6907,7 +7727,7 @@
       <c r="C47" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="13"/>
       <c r="F47" s="2" t="s">
         <v>59</v>
       </c>
@@ -6948,7 +7768,7 @@
       <c r="C48" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E48" s="6"/>
+      <c r="E48" s="13"/>
       <c r="F48" s="2" t="s">
         <v>59</v>
       </c>
@@ -6989,7 +7809,7 @@
       <c r="C49" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="13"/>
       <c r="F49" s="2" t="s">
         <v>69</v>
       </c>
@@ -7033,7 +7853,7 @@
       <c r="D50" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E50" s="13" t="s">
         <v>151</v>
       </c>
       <c r="F50" s="6" t="s">
@@ -7075,22 +7895,22 @@
       <c r="B51" s="2">
         <v>24</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="13" t="s">
         <v>153</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G51" s="9">
         <v>42651</v>
       </c>
-      <c r="K51" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="N51" s="9" t="s">
+      <c r="K51" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N51" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7101,25 +7921,25 @@
       <c r="B52" s="2">
         <v>345</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="13" t="s">
         <v>155</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G52" s="10">
+      <c r="G52" s="9">
         <v>42651</v>
       </c>
-      <c r="K52" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L52" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="P52" s="9" t="s">
+      <c r="K52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P52" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7130,22 +7950,22 @@
       <c r="B53" s="2">
         <v>125</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E53" s="13" t="s">
         <v>157</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G53" s="10">
+      <c r="G53" s="9">
         <v>42651</v>
       </c>
-      <c r="K53" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O53" s="9" t="s">
+      <c r="K53" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="O53" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7156,22 +7976,22 @@
       <c r="B54" s="2">
         <v>28</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E54" s="13" t="s">
         <v>159</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G54" s="10">
+      <c r="G54" s="9">
         <v>42651</v>
       </c>
-      <c r="K54" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O54" s="9" t="s">
+      <c r="K54" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="O54" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7182,7 +8002,7 @@
       <c r="B55" s="2">
         <v>223</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="8" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -7191,10 +8011,10 @@
       <c r="F55" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G55" s="10">
+      <c r="G55" s="9">
         <v>42652</v>
       </c>
-      <c r="S55" s="9" t="s">
+      <c r="S55" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7205,7 +8025,7 @@
       <c r="B56" s="2">
         <v>66</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="8" t="s">
         <v>162</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -7214,10 +8034,10 @@
       <c r="F56" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G56" s="10">
+      <c r="G56" s="9">
         <v>42652</v>
       </c>
-      <c r="S56" s="9" t="s">
+      <c r="S56" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7228,28 +8048,28 @@
       <c r="B57" s="2">
         <v>112</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="8" t="s">
         <v>163</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="13" t="s">
         <v>166</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G57" s="10">
+      <c r="G57" s="9">
         <v>42652</v>
       </c>
-      <c r="Q57" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R57" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z57" s="9" t="s">
+      <c r="Q57" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R57" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z57" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7260,31 +8080,31 @@
       <c r="B58" s="2">
         <v>113</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="8" t="s">
         <v>167</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="13" t="s">
         <v>169</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G58" s="10">
+      <c r="G58" s="9">
         <v>42652</v>
       </c>
-      <c r="M58" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q58" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R58" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z58" s="9" t="s">
+      <c r="M58" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q58" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R58" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z58" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7295,25 +8115,25 @@
       <c r="B59" s="2">
         <v>205</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>171</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="13" t="s">
         <v>172</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G59" s="10">
+      <c r="G59" s="9">
         <v>42653</v>
       </c>
-      <c r="J59" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O59" s="9" t="s">
+      <c r="J59" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="O59" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7324,22 +8144,22 @@
       <c r="B60">
         <v>290</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E60" s="17" t="s">
         <v>174</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G60" s="10">
+      <c r="G60" s="9">
         <v>42653</v>
       </c>
-      <c r="J60" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB60" s="9" t="s">
+      <c r="J60" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB60" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7356,19 +8176,19 @@
       <c r="D61" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="13" t="s">
         <v>177</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G61" s="10">
+      <c r="G61" s="9">
         <v>42653</v>
       </c>
-      <c r="X61" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB61" s="9" t="s">
+      <c r="X61" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB61" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7379,22 +8199,22 @@
       <c r="B62" s="2">
         <v>278</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="E62" s="13" t="s">
         <v>179</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="10">
+      <c r="G62" s="9">
         <v>42653</v>
       </c>
-      <c r="X62" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB62" s="9" t="s">
+      <c r="X62" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB62" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7405,22 +8225,22 @@
       <c r="B63" s="2">
         <v>36</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="E63" s="13" t="s">
         <v>180</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G63" s="10">
+      <c r="G63" s="9">
         <v>42653</v>
       </c>
-      <c r="P63" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB63" s="9" t="s">
+      <c r="P63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB63" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7431,19 +8251,19 @@
       <c r="B64" s="2">
         <v>219</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="8" t="s">
         <v>182</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G64" s="10">
+      <c r="G64" s="9">
         <v>42655</v>
       </c>
-      <c r="J64" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L64" s="9" t="s">
+      <c r="J64" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L64" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7454,16 +8274,16 @@
       <c r="B65" s="2">
         <v>220</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="G65" s="10">
+      <c r="G65" s="9">
         <v>42655</v>
       </c>
     </row>
@@ -7474,7 +8294,7 @@
       <c r="B66" s="2">
         <v>38</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="8" t="s">
         <v>186</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -7483,7 +8303,7 @@
       <c r="F66" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G66" s="10">
+      <c r="G66" s="9">
         <v>42657</v>
       </c>
     </row>
@@ -7494,16 +8314,16 @@
       <c r="B67" s="2">
         <v>58</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E67" s="13" t="s">
         <v>189</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G67" s="10">
+      <c r="G67" s="9">
         <v>42657</v>
       </c>
     </row>
@@ -7514,16 +8334,16 @@
       <c r="B68" s="2">
         <v>14</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="8" t="s">
         <v>190</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G68" s="10">
+      <c r="G68" s="9">
         <v>42658</v>
       </c>
-      <c r="O68" s="13" t="s">
+      <c r="O68" s="11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7534,25 +8354,25 @@
       <c r="B69" s="2">
         <v>198</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="8" t="s">
         <v>191</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E69" s="6" t="s">
+      <c r="E69" s="13" t="s">
         <v>193</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G69" s="10">
+      <c r="G69" s="9">
         <v>42660</v>
       </c>
-      <c r="L69" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC69" s="9" t="s">
+      <c r="L69" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC69" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7563,22 +8383,22 @@
       <c r="B70" s="2">
         <v>303</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="12" t="s">
         <v>195</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G70" s="10">
+      <c r="G70" s="9">
         <v>42660</v>
       </c>
-      <c r="L70" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC70" s="9" t="s">
+      <c r="L70" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC70" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7589,19 +8409,19 @@
       <c r="B71" s="2">
         <v>121</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C71" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="13" t="s">
         <v>198</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G71" s="10">
+      <c r="G71" s="9">
         <v>42660</v>
       </c>
-      <c r="AC71" s="9" t="s">
+      <c r="AC71" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7612,25 +8432,25 @@
       <c r="B72" s="2">
         <v>70</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="8" t="s">
         <v>200</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="13" t="s">
         <v>202</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G72" s="10">
+      <c r="G72" s="9">
         <v>42660</v>
       </c>
-      <c r="S72" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC72" s="9" t="s">
+      <c r="S72" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC72" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7641,22 +8461,22 @@
       <c r="B73" s="2">
         <v>67</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="E73" s="13" t="s">
         <v>204</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G73" s="10">
+      <c r="G73" s="9">
         <v>42661</v>
       </c>
-      <c r="O73" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="S73" s="9" t="s">
+      <c r="O73" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S73" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7667,19 +8487,19 @@
       <c r="B74" s="2">
         <v>396</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="8" t="s">
         <v>205</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G74" s="10">
+      <c r="G74" s="9">
         <v>42661</v>
       </c>
-      <c r="L74" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="S74" s="9" t="s">
+      <c r="L74" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S74" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7690,22 +8510,22 @@
       <c r="B75" s="2">
         <v>155</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C75" s="8" t="s">
         <v>206</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="13" t="s">
         <v>208</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G75" s="10">
+      <c r="G75" s="9">
         <v>42661</v>
       </c>
-      <c r="AA75" s="9" t="s">
+      <c r="AA75" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7719,16 +8539,16 @@
       <c r="C76" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="E76" s="13" t="s">
         <v>210</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G76" s="10">
+      <c r="G76" s="9">
         <v>42662</v>
       </c>
-      <c r="L76" s="9" t="s">
+      <c r="L76" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7739,19 +8559,19 @@
       <c r="B77" s="2">
         <v>414</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G77" s="10">
+      <c r="G77" s="9">
         <v>42662</v>
       </c>
-      <c r="L77" s="9" t="s">
+      <c r="L77" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7762,22 +8582,22 @@
       <c r="B78" s="2">
         <v>240</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="8" t="s">
         <v>213</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="13" t="s">
         <v>217</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G78" s="10">
+      <c r="G78" s="9">
         <v>42663</v>
       </c>
-      <c r="X78" s="9" t="s">
+      <c r="X78" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7788,19 +8608,19 @@
       <c r="B79" s="2">
         <v>35</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="12" t="s">
         <v>219</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G79" s="10">
+      <c r="G79" s="9">
         <v>42664</v>
       </c>
-      <c r="X79" s="9" t="s">
+      <c r="X79" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7817,13 +8637,13 @@
       <c r="F80" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G80" s="10">
+      <c r="G80" s="9">
         <v>42664</v>
       </c>
-      <c r="R80" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X80" s="9" t="s">
+      <c r="R80" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X80" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7834,22 +8654,22 @@
       <c r="B81" s="2">
         <v>74</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="8" t="s">
         <v>222</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="13" t="s">
         <v>224</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G81" s="10">
+      <c r="G81" s="9">
         <v>42664</v>
       </c>
-      <c r="X81" s="9" t="s">
+      <c r="X81" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7863,25 +8683,25 @@
       <c r="C82" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E82" s="6" t="s">
+      <c r="E82" s="13" t="s">
         <v>226</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G82" s="10">
+      <c r="G82" s="9">
         <v>42666</v>
       </c>
-      <c r="Q82" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R82" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="W82" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X82" s="9" t="s">
+      <c r="Q82" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R82" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="W82" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X82" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7898,22 +8718,22 @@
       <c r="D83" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="E83" s="13" t="s">
         <v>229</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G83" s="10">
+      <c r="G83" s="9">
         <v>42667</v>
       </c>
-      <c r="L83" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="S83" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X83" s="9" t="s">
+      <c r="L83" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S83" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X83" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7924,25 +8744,25 @@
       <c r="B84" s="2">
         <v>189</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C84" s="8" t="s">
         <v>230</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="E84" s="13" t="s">
         <v>232</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G84" s="10">
+      <c r="G84" s="9">
         <v>42667</v>
       </c>
-      <c r="K84" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L84" s="9" t="s">
+      <c r="K84" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L84" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7953,22 +8773,22 @@
       <c r="B85" s="2">
         <v>61</v>
       </c>
-      <c r="C85" s="9" t="s">
+      <c r="C85" s="8" t="s">
         <v>233</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="13" t="s">
         <v>234</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G85" s="10">
+      <c r="G85" s="9">
         <v>42667</v>
       </c>
-      <c r="N85" s="9" t="s">
+      <c r="N85" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7982,19 +8802,19 @@
       <c r="C86" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E86" s="13" t="s">
         <v>239</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G86" s="10">
+      <c r="G86" s="9">
         <v>42669</v>
       </c>
-      <c r="X86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC86" s="9" t="s">
+      <c r="X86" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC86" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8008,16 +8828,16 @@
       <c r="C87" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E87" s="6" t="s">
+      <c r="E87" s="13" t="s">
         <v>237</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="G87" s="10">
+      <c r="G87" s="9">
         <v>42669</v>
       </c>
-      <c r="AC87" s="9" t="s">
+      <c r="AC87" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8028,19 +8848,19 @@
       <c r="B88" s="2">
         <v>165</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E88" s="13" t="s">
         <v>241</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G88" s="10">
+      <c r="G88" s="9">
         <v>42670</v>
       </c>
-      <c r="O88" s="9" t="s">
+      <c r="O88" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8051,22 +8871,22 @@
       <c r="B89" s="2">
         <v>338</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C89" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="13" t="s">
         <v>244</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G89" s="10">
+      <c r="G89" s="9">
         <v>42670</v>
       </c>
-      <c r="T89" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC89" s="9" t="s">
+      <c r="T89" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC89" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8077,22 +8897,22 @@
       <c r="B90" s="2">
         <v>319</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="C90" s="8" t="s">
         <v>246</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E90" s="6" t="s">
+      <c r="E90" s="13" t="s">
         <v>247</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G90" s="10">
+      <c r="G90" s="9">
         <v>42672</v>
       </c>
-      <c r="S90" s="9" t="s">
+      <c r="S90" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8103,31 +8923,31 @@
       <c r="B91" s="2">
         <v>268</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C91" s="8" t="s">
         <v>245</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="E91" s="6" t="s">
+      <c r="E91" s="13" t="s">
         <v>248</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G91" s="10">
+      <c r="G91" s="9">
         <v>42672</v>
       </c>
-      <c r="L91" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="S91" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="T91" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X91" s="9" t="s">
+      <c r="L91" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S91" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="T91" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X91" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8144,16 +8964,16 @@
       <c r="D92" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E92" s="13" t="s">
         <v>290</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G92" s="10">
+      <c r="G92" s="9">
         <v>42674</v>
       </c>
-      <c r="AE92" s="9" t="s">
+      <c r="AE92" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8173,10 +8993,10 @@
       <c r="F93" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G93" s="10">
+      <c r="G93" s="9">
         <v>42674</v>
       </c>
-      <c r="AE93" s="9" t="s">
+      <c r="AE93" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8187,22 +9007,22 @@
       <c r="B94" s="2">
         <v>347</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="8" t="s">
         <v>259</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E94" s="6" t="s">
+      <c r="E94" s="13" t="s">
         <v>291</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G94" s="10">
+      <c r="G94" s="9">
         <v>42675</v>
       </c>
-      <c r="AE94" s="9" t="s">
+      <c r="AE94" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8213,19 +9033,19 @@
       <c r="B95" s="2">
         <v>215</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C95" s="8" t="s">
         <v>262</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G95" s="10">
+      <c r="G95" s="9">
         <v>42675</v>
       </c>
-      <c r="V95" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE95" s="9" t="s">
+      <c r="V95" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE95" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8236,25 +9056,25 @@
       <c r="B96" s="2">
         <v>75</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="C96" s="8" t="s">
         <v>263</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="E96" s="13" t="s">
         <v>266</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G96" s="9" t="s">
+      <c r="G96" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="K96" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L96" s="9" t="s">
+      <c r="K96" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L96" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8265,19 +9085,19 @@
       <c r="B97" s="2">
         <v>22</v>
       </c>
-      <c r="C97" s="9" t="s">
+      <c r="C97" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="E97" s="6" t="s">
+      <c r="E97" s="13" t="s">
         <v>271</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G97" s="10">
+      <c r="G97" s="9">
         <v>42681</v>
       </c>
-      <c r="AD97" s="9" t="s">
+      <c r="AD97" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8288,16 +9108,16 @@
       <c r="B98" s="2">
         <v>39</v>
       </c>
-      <c r="C98" s="9" t="s">
+      <c r="C98" s="8" t="s">
         <v>270</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G98" s="10">
+      <c r="G98" s="9">
         <v>42682</v>
       </c>
-      <c r="AD98" s="9" t="s">
+      <c r="AD98" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8308,19 +9128,19 @@
       <c r="B99" s="2">
         <v>40</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C99" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="E99" s="6" t="s">
+      <c r="E99" s="13" t="s">
         <v>273</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G99" s="10">
+      <c r="G99" s="9">
         <v>42683</v>
       </c>
-      <c r="AD99" s="9" t="s">
+      <c r="AD99" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8331,19 +9151,19 @@
       <c r="B100" s="2">
         <v>46</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="C100" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="12" t="s">
         <v>275</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G100" s="10">
+      <c r="G100" s="9">
         <v>42684</v>
       </c>
-      <c r="AD100" s="9" t="s">
+      <c r="AD100" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8354,19 +9174,19 @@
       <c r="B101" s="2">
         <v>47</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C101" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="12" t="s">
         <v>277</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G101" s="10">
+      <c r="G101" s="9">
         <v>42685</v>
       </c>
-      <c r="AD101" s="9" t="s">
+      <c r="AD101" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8377,22 +9197,22 @@
       <c r="B102" s="2">
         <v>92</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C102" s="8" t="s">
         <v>278</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E102" s="6" t="s">
+      <c r="E102" s="13" t="s">
         <v>280</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G102" s="10">
+      <c r="G102" s="9">
         <v>42687</v>
       </c>
-      <c r="N102" s="9" t="s">
+      <c r="N102" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8403,31 +9223,31 @@
       <c r="B103" s="2">
         <v>339</v>
       </c>
-      <c r="C103" s="9" t="s">
+      <c r="C103" s="8" t="s">
         <v>284</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="E103" s="13" t="s">
         <v>91</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G103" s="10">
+      <c r="G103" s="9">
         <v>42699</v>
       </c>
-      <c r="H103" s="14" t="s">
+      <c r="H103" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="I103" t="s">
-        <v>5</v>
-      </c>
-      <c r="R103" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z103" s="9" t="s">
+      <c r="I103" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R103" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z103" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8438,31 +9258,31 @@
       <c r="B104" s="2">
         <v>252</v>
       </c>
-      <c r="C104" s="9" t="s">
+      <c r="C104" s="8" t="s">
         <v>286</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E104" s="6" t="s">
+      <c r="E104" s="13" t="s">
         <v>289</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G104" s="10">
+      <c r="G104" s="9">
         <v>42699</v>
       </c>
-      <c r="H104" s="14" t="s">
+      <c r="H104" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="I104" t="s">
-        <v>5</v>
-      </c>
-      <c r="L104" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="U104" s="9" t="s">
+      <c r="I104" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L104" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="U104" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8473,25 +9293,25 @@
       <c r="B105" s="2">
         <v>266</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="8" t="s">
         <v>295</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="E105" s="2" t="s">
+      <c r="E105" s="13" t="s">
         <v>297</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G105" s="10">
+      <c r="G105" s="9">
         <v>42700</v>
       </c>
-      <c r="H105" s="15" t="s">
+      <c r="H105" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="I105" t="s">
+      <c r="I105" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8502,7 +9322,7 @@
       <c r="B106" s="2">
         <v>243</v>
       </c>
-      <c r="C106" s="9" t="s">
+      <c r="C106" s="8" t="s">
         <v>299</v>
       </c>
       <c r="D106" s="2" t="s">
@@ -8511,16 +9331,16 @@
       <c r="F106" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G106" s="10">
+      <c r="G106" s="9">
         <v>42700</v>
       </c>
-      <c r="H106" s="9" t="s">
+      <c r="H106" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="I106" t="s">
-        <v>5</v>
-      </c>
-      <c r="L106" s="9" t="s">
+      <c r="I106" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L106" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8531,7 +9351,7 @@
       <c r="B107" s="2">
         <v>246</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="8" t="s">
         <v>301</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -8540,16 +9360,16 @@
       <c r="F107" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G107" s="10">
+      <c r="G107" s="9">
         <v>42700</v>
       </c>
-      <c r="H107" s="9" t="s">
+      <c r="H107" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="I107" t="s">
-        <v>5</v>
-      </c>
-      <c r="J107" s="9" t="s">
+      <c r="I107" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J107" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8560,28 +9380,28 @@
       <c r="B108" s="2">
         <v>276</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="C108" s="8" t="s">
         <v>302</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E108" s="9" t="s">
+      <c r="E108" s="12" t="s">
         <v>304</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="G108" s="10">
+      <c r="G108" s="9">
         <v>42700</v>
       </c>
-      <c r="H108" s="9" t="s">
+      <c r="H108" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="I108" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC108" s="9" t="s">
+      <c r="I108" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC108" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8592,31 +9412,31 @@
       <c r="B109" s="2">
         <v>270</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C109" s="8" t="s">
         <v>306</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="E109" s="6" t="s">
+      <c r="E109" s="13" t="s">
         <v>310</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="G109" s="10">
+      <c r="G109" s="9">
         <v>42701</v>
       </c>
-      <c r="H109" s="9" t="s">
+      <c r="H109" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="I109" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q109" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X109" s="9" t="s">
+      <c r="I109" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q109" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X109" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8627,22 +9447,22 @@
       <c r="B110" s="2">
         <v>170</v>
       </c>
-      <c r="C110" s="9" t="s">
+      <c r="C110" s="8" t="s">
         <v>308</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E110" s="2" t="s">
+      <c r="E110" s="13" t="s">
         <v>317</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="G110" s="10">
+      <c r="G110" s="9">
         <v>42701</v>
       </c>
-      <c r="H110" s="9" t="s">
+      <c r="H110" s="8" t="s">
         <v>283</v>
       </c>
     </row>
@@ -8653,31 +9473,31 @@
       <c r="B111" s="2">
         <v>167</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="C111" s="8" t="s">
         <v>318</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="E111" s="13" t="s">
         <v>320</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G111" s="10">
+      <c r="G111" s="9">
         <v>42623</v>
       </c>
-      <c r="H111" s="9" t="s">
+      <c r="H111" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="K111" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L111" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X111" s="9" t="s">
+      <c r="K111" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L111" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X111" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8688,115 +9508,115 @@
       <c r="B112" s="2">
         <v>280</v>
       </c>
-      <c r="C112" s="9" t="s">
+      <c r="C112" s="8" t="s">
         <v>322</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="E112" s="13" t="s">
         <v>325</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G112" s="10">
+      <c r="G112" s="9">
         <v>42701</v>
       </c>
-      <c r="H112" s="9" t="s">
+      <c r="H112" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="I112" t="s">
-        <v>5</v>
-      </c>
-      <c r="L112" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="U112" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:30" ht="204" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I112" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L112" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="U112" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:32" ht="204" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B113" s="2">
         <v>366</v>
       </c>
-      <c r="C113" s="9" t="s">
+      <c r="C113" s="8" t="s">
         <v>329</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="E113" s="17" t="s">
+      <c r="E113" s="13" t="s">
         <v>327</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G113" s="10">
+      <c r="G113" s="9">
         <v>42702</v>
       </c>
-      <c r="H113" s="9" t="s">
+      <c r="H113" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="Q113" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z113" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD113" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="114" spans="1:30" ht="261" x14ac:dyDescent="0.35">
+      <c r="Q113" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z113" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD113" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:32" ht="261" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B114" s="2">
         <v>364</v>
       </c>
-      <c r="C114" s="9" t="s">
+      <c r="C114" s="8" t="s">
         <v>330</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E114" s="2" t="s">
+      <c r="E114" s="13" t="s">
         <v>336</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G114" s="10">
+      <c r="G114" s="9">
         <v>42705</v>
       </c>
-      <c r="H114" s="9" t="s">
+      <c r="H114" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="R114" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z114" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:30" ht="261" x14ac:dyDescent="0.35">
+      <c r="R114" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z114" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:32" ht="261" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B115" s="2">
         <v>249</v>
       </c>
-      <c r="C115" s="9" t="s">
+      <c r="C115" s="8" t="s">
         <v>332</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E115" s="17" t="s">
         <v>335</v>
       </c>
       <c r="F115" s="2" t="s">
@@ -8808,223 +9628,229 @@
       <c r="I115" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="116" spans="1:30" ht="116" x14ac:dyDescent="0.35">
+      <c r="J115" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB115" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:32" ht="116" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B116" s="2">
         <v>320</v>
       </c>
-      <c r="C116" s="9" t="s">
+      <c r="C116" s="8" t="s">
         <v>337</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="E116" s="6" t="s">
+      <c r="E116" s="13" t="s">
         <v>339</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G116" s="10">
+      <c r="G116" s="9">
         <v>42708</v>
       </c>
-      <c r="H116" s="9" t="s">
+      <c r="H116" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="I116" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD116" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:30" ht="288.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I116" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD116" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:32" ht="288.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B117" s="2">
         <v>254</v>
       </c>
-      <c r="C117" s="9" t="s">
+      <c r="C117" s="8" t="s">
         <v>340</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="E117" s="17" t="s">
+      <c r="E117" s="18" t="s">
         <v>343</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G117" s="10">
+      <c r="G117" s="9">
         <v>42709</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="I117" t="s">
-        <v>5</v>
-      </c>
-      <c r="R117" s="9" t="s">
+      <c r="I117" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R117" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="AD117" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:30" ht="145" x14ac:dyDescent="0.35">
+      <c r="AD117" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:32" ht="145" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B118" s="2">
         <v>131</v>
       </c>
-      <c r="C118" s="9" t="s">
+      <c r="C118" s="8" t="s">
         <v>345</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="E118" s="6" t="s">
+      <c r="E118" s="13" t="s">
         <v>347</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G118" s="10">
+      <c r="G118" s="9">
         <v>42716</v>
       </c>
-      <c r="H118" s="9" t="s">
+      <c r="H118" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="M118" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R118" s="9" t="s">
+      <c r="M118" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R118" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="AD118" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:30" ht="149" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AD118" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:32" ht="149" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B119" s="2">
         <v>89</v>
       </c>
-      <c r="C119" s="9" t="s">
+      <c r="C119" s="8" t="s">
         <v>348</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="E119" s="6" t="s">
+      <c r="E119" s="13" t="s">
         <v>350</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G119" s="10">
+      <c r="G119" s="9">
         <v>42718</v>
       </c>
-      <c r="H119" s="9" t="s">
+      <c r="H119" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="T119" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="120" spans="1:30" ht="174" x14ac:dyDescent="0.35">
+      <c r="T119" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:32" ht="174" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B120" s="2">
         <v>77</v>
       </c>
-      <c r="C120" s="9" t="s">
+      <c r="C120" s="8" t="s">
         <v>352</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="E120" s="6" t="s">
+      <c r="E120" s="13" t="s">
         <v>356</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G120" s="10">
+      <c r="G120" s="9">
         <v>42718</v>
       </c>
-      <c r="AD120" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="121" spans="1:30" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="AD120" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:32" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B121" s="2">
         <v>216</v>
       </c>
-      <c r="C121" s="9" t="s">
+      <c r="C121" s="8" t="s">
         <v>353</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="E121" s="6" t="s">
+      <c r="E121" s="13" t="s">
         <v>356</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G121" s="10">
+      <c r="G121" s="9">
         <v>42719</v>
       </c>
-      <c r="L121" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD121" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:30" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="L121" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD121" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:32" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B122" s="2">
         <v>60</v>
       </c>
-      <c r="C122" s="9" t="s">
+      <c r="C122" s="8" t="s">
         <v>357</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="E122" s="6" t="s">
+      <c r="E122" s="13" t="s">
         <v>359</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="G122" s="10">
+      <c r="G122" s="9">
         <v>42719</v>
       </c>
-      <c r="N122" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD122" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="123" spans="1:30" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="N122" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD122" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:32" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>46</v>
       </c>
@@ -9037,58 +9863,58 @@
       <c r="D123" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="E123" s="6" t="s">
+      <c r="E123" s="13" t="s">
         <v>365</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G123" s="10">
+      <c r="G123" s="9">
         <v>42723</v>
       </c>
       <c r="H123" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="O123" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD123" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="124" spans="1:30" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="O123" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD123" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:32" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B124" s="2">
         <v>79</v>
       </c>
-      <c r="C124" s="9" t="s">
+      <c r="C124" s="8" t="s">
         <v>367</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="E124" s="13" t="s">
         <v>369</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="G124" s="10">
+      <c r="G124" s="9">
         <v>42723</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="L124" s="9" t="s">
+      <c r="L124" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="AD124" s="9" t="s">
+      <c r="AD124" s="8" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="125" spans="1:30" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:32" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>46</v>
       </c>
@@ -9096,27 +9922,341 @@
         <v>357</v>
       </c>
       <c r="C125" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D125" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D125" s="2" t="s">
+      <c r="E125" s="13" t="s">
         <v>371</v>
-      </c>
-      <c r="E125" s="6" t="s">
-        <v>372</v>
       </c>
       <c r="F125" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G125" s="10">
+      <c r="G125" s="9">
         <v>42723</v>
       </c>
-      <c r="H125" s="9" t="s">
+      <c r="H125" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="AC125" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD125" s="9" t="s">
+      <c r="AC125" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD125" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:32" ht="87" x14ac:dyDescent="0.35">
+      <c r="A126" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B126" s="2">
+        <v>346</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E126" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G126" s="9">
+        <v>42723</v>
+      </c>
+      <c r="H126" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="I126" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA126" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF126" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:32" ht="145" x14ac:dyDescent="0.35">
+      <c r="A127" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B127" s="2">
+        <v>288</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E127" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G127" s="9">
+        <v>42723</v>
+      </c>
+      <c r="H127" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="I127" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J127" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF127" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:32" ht="232" x14ac:dyDescent="0.35">
+      <c r="A128" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B128" s="2">
+        <v>392</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E128" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G128" s="9">
+        <v>42724</v>
+      </c>
+      <c r="H128" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="O128" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A129" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B129" s="2">
+        <v>153</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E129" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G129" s="9">
+        <v>42724</v>
+      </c>
+      <c r="H129" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="L129" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X129" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:24" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A130" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B130" s="2">
+        <v>274</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E130" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G130" s="9">
+        <v>42724</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="L130" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="U130" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:24" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A131" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B131" s="2">
+        <v>275</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E131" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G131" s="9">
+        <v>42724</v>
+      </c>
+      <c r="H131" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="L131" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X131" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:24" ht="290" x14ac:dyDescent="0.35">
+      <c r="A132" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B132" s="2">
+        <v>475</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E132" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G132" s="9">
+        <v>42724</v>
+      </c>
+      <c r="H132" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="K132" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q132" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:24" ht="58" x14ac:dyDescent="0.35">
+      <c r="A133" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B133" s="2">
+        <v>50</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G133" s="9">
+        <v>42725</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="S133" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+      <c r="A134" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B134" s="2">
+        <v>242</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E134" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G134" s="9">
+        <v>42725</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="J134" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P134" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:24" ht="203" x14ac:dyDescent="0.35">
+      <c r="A135" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B135" s="2">
+        <v>438</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E135" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G135" s="9">
+        <v>42725</v>
+      </c>
+      <c r="H135" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="O135" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -9129,10 +10269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E7"/>
+  <dimension ref="B1:E9"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9157,7 +10297,7 @@
       </c>
     </row>
     <row r="2" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>132</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -9165,7 +10305,7 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>135</v>
       </c>
     </row>
@@ -9199,6 +10339,16 @@
       </c>
       <c r="C7" s="6" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5 for Jan 11
</commit_message>
<xml_diff>
--- a/Leetcode record for Shiyun.xlsx
+++ b/Leetcode record for Shiyun.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="670">
   <si>
     <t>Two Pointers</t>
   </si>
@@ -2271,9 +2271,6 @@
     <t>Turn off bit</t>
   </si>
   <si>
-    <t>&amp; with 1</t>
-  </si>
-  <si>
     <t>&gt;&gt;&gt;</t>
   </si>
   <si>
@@ -2284,12 +2281,6 @@
   </si>
   <si>
     <t>signed shift (the first bit stays the same)</t>
-  </si>
-  <si>
-    <t>Set bit /turn on</t>
-  </si>
-  <si>
-    <t>| 1</t>
   </si>
   <si>
     <t>This is more of a combination problem rather than permutation. So if each time search from the beginning it is slow, use binary number to keep track of what's used. The number represent the track we have visited before, and will be used as the key of map
@@ -3651,12 +3642,6 @@
 2. Reverse each word.</t>
   </si>
   <si>
-    <t>str.split(" ")
-String[] parts = s.trim().split("\\s+"); //remove multiple spaces
-str.lastIndexOf("a")
-String s = new String(charArray); //convert char array back to a String</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">.values() returns a Collections of values. (Collections is the super class of List) 
 </t>
@@ -3816,6 +3801,383 @@
 solution.pick(3);
 // pick(1) should return 0. Since in the array only nums[0] is equal to 1.
 solution.pick(1);</t>
+  </si>
+  <si>
+    <t>Steps:
+1. Compare right and left heights, move the shorter one to next (because moving bigger one will only make area smaller because x is shorter but y is the same)
+2. Stores all areas in each case in list
+3. Pick the max area from the list</t>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>Given n non-negative integers a1, a2, ..., an, where each represents a point at coordinate (i, ai). n vertical lines are drawn such that the two endpoints of line i is at (i, ai) and (i, 0). Find two lines, which together with x-axis forms a container, such that the container contains the most water.
+Note: You may not slant the container and n is at least 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google 
+Twitter 
+Zenefits 
+Amazon 
+Apple 
+Bloomberg </t>
+  </si>
+  <si>
+    <t>Corner case:
+[5,2,1,2,1,5]
+Method 1: a stack of decreasing heights, when increase, pop() as bottom, peek() as left height (when not empty)
+Method 2: 2 pointers from left and right, for each index, the water that fit is min of 2 pointers' height minus index height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given n non-negative integers representing an elevation map where the width of each bar is 1, compute how much water it is able to trap after raining.
+For example, 
+Given [0,1,0,2,1,0,1,3,2,1,2,1], return 6.
+</t>
+  </si>
+  <si>
+    <t>Trapping Rain Water</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array II</t>
+  </si>
+  <si>
+    <t>Follow up for "Remove Duplicates":
+What if duplicates are allowed at most twice?
+For example,
+Given sorted array nums = [1,1,1,2,2,3],
+Your function should return length = 5, with the first five elements of nums being 1, 1, 2, 2 and 3. It doesn't matter what you leave beyond the new length.</t>
+  </si>
+  <si>
+    <t>Steps:
+1. Two pointers, one is res, one is i for looping whole array
+2. The idea is res only ++ when the num should be kept, but i always ++, so if there are unwanted number, i will be larger than res, those between i and res are numbers to be throws away, they will be replace when res++
+3. When the num is legal, copy nums[i] to nums[res];</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>public static int binarySearch(int[] a,
+               int fromIndex,
+               int toIndex,
+               int key)
+Returns:
+index of the search key, if it is contained in the array within the specified range; otherwise, (-(insertion point) - 1). This guarantees that the return value will be &gt;= 0 if and only if the key is found.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Needs to judge:
+1. which part is sorted
+2. target compare with nums[mid]
+3. if nums[right] == nums[left] == nums[mid], can only move pointers now
+Corner cases:
+1. [1,3,5] find 1 //Arrays.binarySearch returns </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;= 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when found, not &gt; 0, also end index is exclusive
+2. [1,1,3,1] find 3
+3. [3,1,1] find 3</t>
+    </r>
+  </si>
+  <si>
+    <t>Beat 70% 依旧注意Arrays.binarySearch() 返回&gt;= 0</t>
+  </si>
+  <si>
+    <t>Suppose an array sorted in ascending order is rotated at some pivot unknown to you beforehand.
+(i.e., 0 1 2 4 5 6 7 might become 4 5 6 7 0 1 2).
+You are given a target value to search. If found in the array return its index, otherwise return -1.
+You may assume no duplicate exists in the array.</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Follow up for "Search in Rotated Sorted Array":
+What if duplicates are allowed?
+Would this affect the run-time complexity? How and why?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yes, worst case O(n), consider 1,1,1,1,1,1,1,1,5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Suppose an array sorted in ascending order is rotated at some pivot unknown to you beforehand.
+(i.e., 0 1 2 4 5 6 7 might become 4 5 6 7 0 1 2).
+Write a function to determine if a given target is in the array.
+The array may contain duplicates.</t>
+    </r>
+  </si>
+  <si>
+    <t>Spiral Matrix</t>
+  </si>
+  <si>
+    <t>Given a matrix of m x n elements (m rows, n columns), return all elements of the matrix in spiral order.
+For example,
+Given the following matrix:
+[
+ [ 1, 2, 3 ],
+ [ 4, 5, 6 ],
+ [ 7, 8, 9 ]
+]
+You should return [1,2,3,6,9,8,7,4,5].</t>
+  </si>
+  <si>
+    <t>Avoid walking the same path. To do so, compare up/down or lft/rgt everytime they changes.</t>
+  </si>
+  <si>
+    <t>Find the total Hamming distance between all pairs of the given numbers.
+Example:
+Input: 4, 14, 2
+Output: 6
+Explanation: In binary representation, the 4 is 0100, 14 is 1110, and 2 is 0010 (just showing the four bits relevant in this case). So the answer will be:
+HammingDistance(4, 14) + HammingDistance(4, 2) + HammingDistance(14, 2) = 2 + 2 + 2 = 6.
+Note:
+Elements of the given array are in the range of 0 to 10^9
+Length of the array will not exceed 10^4.</t>
+  </si>
+  <si>
+    <t>Assuming we have an array of five integers a, b, c, d, e as follow.
+We examine the digits one by one from the last digit.
+Count the number of integers whose last digit is 1, assign the value to ones
+    a = 0 0 0 1 0
+    b = 1 0 0 1 1
+    c = 0 1 0 0 1
+    d = 1 0 0 1 0
+    e = 0 0 0 1 0
+                       ↑
+    ones: b, c
+    zeros: a, d, e
+    So we have 2 ones and 5 - 2 = 3 zeros
+    Total distance = 2 * 3
+    then we move the pointer one position left, i.e. all the numbers right shift by 1 (num &gt;&gt;&gt; 1)</t>
+  </si>
+  <si>
+    <t>Spiral Matrix II</t>
+  </si>
+  <si>
+    <t>Given an integer n, generate a square matrix filled with elements from 1 to n2 in spiral order.
+For example,
+Given n = 3,
+You should return the following matrix:
+[
+ [ 1, 2, 3 ],
+ [ 8, 9, 4 ],
+ [ 7, 6, 5 ]
+]</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>Given a m x n matrix, if an element is 0, set its entire row and column to 0. Do it in place.
+Follow up:
+Did you use extra space?
+A straight forward solution using O(mn) space is probably a bad idea.
+A simple improvement uses O(m + n) space, but still not the best solution.
+Could you devise a constant space solution?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My O(m + n) space solution, just loop through all elements, put empty rows and cols indices in a set, then loop through set to set 0 in original matrix.
+An O(1) space solution is use first row and first column as markers of 0, also keep 2 boolean indicating whether first col and first row need to be set to 0. </t>
+  </si>
+  <si>
+    <t>Game of Life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkedIn 
+Bloomberg 
+Uber 
+Facebook 
+Microsoft </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft 
+Google 
+Uber </t>
+  </si>
+  <si>
+    <t>Microsoft
+Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropbox 
+Google 
+Two Sigma 
+Snapchat </t>
+  </si>
+  <si>
+    <t>Set bit /turn on (make it 1)</t>
+  </si>
+  <si>
+    <t>invert a specific bit</t>
+  </si>
+  <si>
+    <t>myByte ^= 1 &lt;&lt; bit;</t>
+  </si>
+  <si>
+    <t>| 1
+myByte |= 1 &lt;&lt; pos;</t>
+  </si>
+  <si>
+    <t>&amp; with 1
+myByte &amp;= ~(1 &lt;&lt; position);</t>
+  </si>
+  <si>
+    <t>Given a board with m by n cells, each cell has an initial state live (1) or dead (0). Each cell interacts with its eight neighbors (horizontal, vertical, diagonal) using the following four rules (taken from the above Wikipedia article):
+Any live cell with fewer than two live neighbors dies, as if caused by under-population.
+Any live cell with two or three live neighbors lives on to the next generation.
+Any live cell with more than three live neighbors dies, as if by over-population..
+Any dead cell with exactly three live neighbors becomes a live cell, as if by reproduction.
+Write a function to compute the next state (after one update) of the board given its current state.</t>
+  </si>
+  <si>
+    <t>In place and bit-manipulation steps:
+1. A separate method to calculate neighbors, calculate the 3 * 3 grids then minus itself. Tricky parts: termination is &lt;= not &lt;, in the end minus res itself, remember to &amp; 1
+2. Use 2 bits to represent next state and current state, next state is default to be 0
+3. To get the current state, board[i][j] &amp; 1
+To get the next state, board[i][j] &gt;&gt; 1
+Follow up: 
+Could you solve it in-place? Remember that the board needs to be updated at the same time: You cannot update some cells first and then use their updated values to update other cells.
+In this question, we represent the board using a 2D array. In principle, the board is infinite, which would cause problems when the active area encroaches the border of the array. How would you address these problems?</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Integer.parseInt(String str);//return Integer
+Integer.valueOf(String str);//return Integer</t>
+  </si>
+  <si>
+    <t>Summary Ranges</t>
+  </si>
+  <si>
+    <t>str.split(" ")
+String[] parts = s.trim().split("\\s+"); //remove multiple spaces
+str.lastIndexOf("a")
+String s = new String(charArray); //convert char array back to a String
+String.valueOf(Integer); 或 String.toString(int)//return String</t>
+  </si>
+  <si>
+    <t>Given a sorted integer array without duplicates, return the summary of its ranges.
+For example, given [0,1,2,4,5,7], return ["0-&gt;2","4-&gt;5","7"].</t>
+  </si>
+  <si>
+    <t>Corner case: 
+1. only 1 number in the array
+2. [1,3]
+3. [-2147483648,-2147483647,2147483647]
+Steps:
+1. Start from i = 0 is better than ii = 1, careful for int overflow when nums[i + 1] - nums[i], so nums[i] + 1 == nums[i + 1] is better.
+2. Take care of the final element in the array (start from i = 0 can do it)</t>
+  </si>
+  <si>
+    <t>Minimum Size Subarray Sum</t>
+  </si>
+  <si>
+    <t>Given an array of n positive integers and a positive integer s, find the minimal length of a contiguous subarray of which the sum ≥ s. If there isn't one, return 0 instead.
+For example, given the array [2,3,1,2,4,3] and s = 7,
+the subarray [4,3] has the minimal length under the problem constraint.
+If you have figured out the O(n) solution, try coding another solution of which the time complexity is O(n log n).</t>
+  </si>
+  <si>
+    <t>Corner cases:
+1. input array is empty, return 0
+2. if all element in array add up is less than target, return 0
+3. 213 [12,28,83,4,25,26,25,2,25,25,25,12] //return 8
+4. 11 [1,2,3,4,5] //return 3
+In conclusion, need to consider when adding all is smaller than target, the final one in the array
+Let sum be 0 at first and add nums[b] before b++ will save some effort
+Basic idea is to use two pointers, when sum &gt;= target, move left pointer, else move right</t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
+    <t>就是一个循环（没有嵌套），两个不嵌套的循环还是算O(n)</t>
+  </si>
+  <si>
+    <t>Given an array of integers where 1 ≤ a[i] ≤ n (n = size of array), some elements appear twice and others appear once.
+Find all the elements of [1, n] inclusive that do not appear in this array.
+Could you do it without extra space and in O(n) runtime? You may assume the returned list does not count as extra space.
+Example:
+Input:
+[4,3,2,7,8,2,3,1]
+Output:
+[5,6]</t>
+  </si>
+  <si>
+    <t>Find All Numbers Disappeared in an Array</t>
+  </si>
+  <si>
+    <t>Corner Case:
+1. [1,1] 缺结尾到n
+2. empty array input
+3. [2,2] 缺1到开头
+Negative number marker method
+1. iterate once, when meet a num in arr, mark arr[num] to be negative if not already. 
+2. iterate second time, if number not negative, add the index to list.
+(base on the fact that all numbers in the arr are &lt;= arr.length</t>
+  </si>
+  <si>
+    <t>Assign Cookies</t>
+  </si>
+  <si>
+    <t>Corner case:
+[10,9,8,7]
+[5,6,7,8]
+Steps:
+1. sort two arrays
+2. two pointers for each of them, move child pointer when one is content</t>
+  </si>
+  <si>
+    <t>Assume you are an awesome parent and want to give your children some cookies. But, you should give each child at most one cookie. Each child i has a greed factor gi, which is the minimum size of a cookie that the child will be content with; and each cookie j has a size sj. If sj &gt;= gi, we can assign the cookie j to the child i, and the child i will be content. Your goal is to maximize the number of your content children and output the maximum number.
+Note:
+You may assume the greed factor is always positive. 
+You cannot assign more than one cookie to one child.
+Example 1:
+Input: [1,2,3], [1,1]
+Output: 1</t>
   </si>
 </sst>
 </file>
@@ -6026,8 +6388,8 @@
       <xdr:row>167</xdr:row>
       <xdr:rowOff>1139229</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId66">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Ink 15">
@@ -6046,7 +6408,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Ink 15">
@@ -6091,8 +6453,8 @@
       <xdr:row>167</xdr:row>
       <xdr:rowOff>1134189</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId68">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="18" name="Ink 17">
@@ -6111,7 +6473,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="18" name="Ink 17">
@@ -6156,8 +6518,8 @@
       <xdr:row>167</xdr:row>
       <xdr:rowOff>1324509</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId70">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="19" name="Ink 18">
@@ -6176,7 +6538,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="19" name="Ink 18">
@@ -6221,8 +6583,8 @@
       <xdr:row>167</xdr:row>
       <xdr:rowOff>1578669</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId72">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="20" name="Ink 19">
@@ -6241,7 +6603,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="20" name="Ink 19">
@@ -6286,8 +6648,8 @@
       <xdr:row>167</xdr:row>
       <xdr:rowOff>1587789</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId74">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="23" name="Ink 22">
@@ -6306,7 +6668,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="23" name="Ink 22">
@@ -6351,8 +6713,8 @@
       <xdr:row>167</xdr:row>
       <xdr:rowOff>1765149</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId76">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="28" name="Ink 27">
@@ -6371,7 +6733,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="28" name="Ink 27">
@@ -6477,8 +6839,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2566618</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId79">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="35" name="Ink 34">
@@ -6497,7 +6859,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="35" name="Ink 34">
@@ -6542,8 +6904,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>1767898</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId81">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="40" name="Ink 39">
@@ -6562,7 +6924,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="40" name="Ink 39">
@@ -6607,8 +6969,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2143498</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId83">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="42" name="Ink 41">
@@ -6627,7 +6989,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="42" name="Ink 41">
@@ -6672,8 +7034,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2426218</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId85">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="46" name="Ink 45">
@@ -6692,7 +7054,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="46" name="Ink 45">
@@ -6737,8 +7099,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2374858</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId87">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="47" name="Ink 46">
@@ -6757,7 +7119,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="47" name="Ink 46">
@@ -6802,8 +7164,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2401738</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId89">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="49" name="Ink 48">
@@ -6822,7 +7184,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="49" name="Ink 48">
@@ -6867,8 +7229,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2466298</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId91">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="54" name="Ink 53">
@@ -6887,7 +7249,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="54" name="Ink 53">
@@ -6932,8 +7294,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2446138</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId93">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="60" name="Ink 59">
@@ -6952,7 +7314,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="60" name="Ink 59">
@@ -6997,8 +7359,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2038618</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId95">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="62" name="Ink 61">
@@ -7017,7 +7379,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="62" name="Ink 61">
@@ -7062,8 +7424,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2651818</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId97">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="64" name="Ink 63">
@@ -7082,7 +7444,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="64" name="Ink 63">
@@ -7127,8 +7489,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2494378</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId99">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="108" name="Ink 107">
@@ -7147,7 +7509,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="108" name="Ink 107">
@@ -7192,8 +7554,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>1998298</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId101">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="111" name="Ink 110">
@@ -7212,7 +7574,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="111" name="Ink 110">
@@ -7257,8 +7619,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2301658</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId103">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="122" name="Ink 121">
@@ -7277,7 +7639,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="122" name="Ink 121">
@@ -7322,8 +7684,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>428218</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId105">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="132" name="Ink 131">
@@ -7342,7 +7704,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="132" name="Ink 131">
@@ -7387,8 +7749,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>1493578</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId107">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="135" name="Ink 134">
@@ -7407,7 +7769,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="135" name="Ink 134">
@@ -7452,8 +7814,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2324098</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId109">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="136" name="Ink 135">
@@ -7472,7 +7834,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="136" name="Ink 135">
@@ -7517,8 +7879,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>1559458</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId111">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="137" name="Ink 136">
@@ -7537,7 +7899,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="137" name="Ink 136">
@@ -7582,8 +7944,8 @@
       <xdr:row>170</xdr:row>
       <xdr:rowOff>2737018</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId113">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="138" name="Ink 137">
@@ -7602,7 +7964,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="138" name="Ink 137">
@@ -7624,6 +7986,841 @@
             <a:xfrm>
               <a:off x="8259720" y="235919160"/>
               <a:ext cx="1382040" cy="729720"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>30186</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>1280324</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4150309</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>2741342</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Picture 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{947F56CD-A9CE-46BF-9261-099A4C629B93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId115" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6313072" y="271764511"/>
+          <a:ext cx="4120123" cy="1461018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>938390</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>1467055</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3081917</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>3308023</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{664B624C-E143-4675-BAA0-C124F06068D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId116" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect b="16119"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7217834" y="274834555"/>
+          <a:ext cx="2143527" cy="1840968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1379593</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>1511749</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2200033</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2043469</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId117">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19DF58B0-68F4-490E-8D95-086A3B1117BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7660320" y="278775840"/>
+            <a:ext cx="820440" cy="531720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19DF58B0-68F4-490E-8D95-086A3B1117BC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId118"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7656000" y="278771520"/>
+              <a:ext cx="829080" cy="540360"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2429833</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2037589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3181153</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2609989</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId119">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F926AACC-B4FF-4B89-8A78-C4BF992D201A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8710560" y="279301680"/>
+            <a:ext cx="751320" cy="572400"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F926AACC-B4FF-4B89-8A78-C4BF992D201A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId120"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8706240" y="279297360"/>
+              <a:ext cx="759960" cy="581040"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1771993</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>1685509</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1899433</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>1796869</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId121">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="17" name="Ink 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0AA7E4F-7CBB-41E3-A80F-B9417F42FB2D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8052720" y="278949600"/>
+            <a:ext cx="127440" cy="111360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="17" name="Ink 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0AA7E4F-7CBB-41E3-A80F-B9417F42FB2D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId122"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8048400" y="278945275"/>
+              <a:ext cx="136080" cy="120009"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1829833</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>1385269</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1927393</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>10051</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId123">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="22" name="Ink 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C2EE4C4-C7CF-45C2-8B61-0C80DE6CC9CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8110560" y="278649360"/>
+            <a:ext cx="97560" cy="1245600"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="22" name="Ink 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C2EE4C4-C7CF-45C2-8B61-0C80DE6CC9CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId124"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8106240" y="278645040"/>
+              <a:ext cx="106200" cy="1254240"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2823913</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2210869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2928553</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2319589</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId125">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFEFEE9C-75C9-4A5F-9DE2-EA3DDF0A12A1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9104640" y="279474960"/>
+            <a:ext cx="104640" cy="108720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFEFEE9C-75C9-4A5F-9DE2-EA3DDF0A12A1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId126"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9100325" y="279470640"/>
+              <a:ext cx="113270" cy="117360"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2869033</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>1702789</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2887033</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2465269</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId127">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="32" name="Ink 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92D744DD-4643-4940-B04C-BA77EEA04627}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9149760" y="278966880"/>
+            <a:ext cx="18000" cy="762480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="32" name="Ink 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92D744DD-4643-4940-B04C-BA77EEA04627}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId128"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9145440" y="278962560"/>
+              <a:ext cx="26640" cy="771120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1408393</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2043349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1571833</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2043589</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId129">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="37" name="Ink 36">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADB24EE7-2765-443D-B50B-5F86C703D484}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7689120" y="279307440"/>
+            <a:ext cx="163440" cy="240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="37" name="Ink 36">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADB24EE7-2765-443D-B50B-5F86C703D484}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId130"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7684800" y="279304560"/>
+              <a:ext cx="172080" cy="6000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2886313</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2031829</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3256393</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2038069</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId131">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="51" name="Ink 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75C99B06-90DA-4E75-814C-15C90482AF2B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9167040" y="279295920"/>
+            <a:ext cx="370080" cy="6240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="51" name="Ink 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75C99B06-90DA-4E75-814C-15C90482AF2B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId132"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9162720" y="279291760"/>
+              <a:ext cx="378720" cy="14560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2505193</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2014549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2616793</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2014789</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId133">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="52" name="Ink 51">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11CAC76E-E841-456B-814E-7EBDDA232397}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8785920" y="279278640"/>
+            <a:ext cx="111600" cy="240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="52" name="Ink 51">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11CAC76E-E841-456B-814E-7EBDDA232397}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId134"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8781600" y="279275760"/>
+              <a:ext cx="120240" cy="6000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2176153</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2037589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2343193</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2038069</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId135">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="56" name="Ink 55">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60002C66-353E-453E-9E18-0CF89B61E78C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8456880" y="279301680"/>
+            <a:ext cx="167040" cy="480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="56" name="Ink 55">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60002C66-353E-453E-9E18-0CF89B61E78C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId136"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8452560" y="279298800"/>
+              <a:ext cx="175680" cy="6240"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1789513</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2043349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1989913</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>2049349</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId137">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="61" name="Ink 60">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2E2920-AAA3-44BE-AE89-AB83A130CA8A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8070240" y="279307440"/>
+            <a:ext cx="200400" cy="6000"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="61" name="Ink 60">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2E2920-AAA3-44BE-AE89-AB83A130CA8A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId138"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8065923" y="279303205"/>
+              <a:ext cx="209035" cy="14471"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8839,7 +10036,7 @@
     <inkml:annotationXML>
       <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
         <emma:interpretation id="{B1E1B447-3FB1-47A5-8381-5E38BC4AD189}" emma:medium="tactile" emma:mode="ink">
-          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="19331,573349 24450,573627 24421,574166 19302,573889" semanticType="10" shapeName="Other">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="19331,573349 24450,573627 24421,574166 19302,573889" semanticType="underline" shapeName="Other">
             <msink:sourceLink direction="with" ref="{44B80033-1300-4851-89A8-EDB4FC5BB013}"/>
             <msink:sourceLink direction="with" ref="{B3449365-B854-4E1F-BFF3-8274CD38744A}"/>
           </msink:context>
@@ -9813,16 +11010,16 @@
       <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
         <emma:interpretation id="{D27276A3-85C1-4C5A-A1BF-EA78209F48FF}" emma:medium="tactile" emma:mode="ink">
           <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="19668,653198 27099,652942 27235,656865 19804,657122" semanticType="enclosure" shapeName="Other">
+            <msink:sourceLink direction="with" ref="{63583EF9-AB05-429F-ACBA-B6DF15FB3804}"/>
             <msink:sourceLink direction="with" ref="{725D1255-EB1C-43CB-9B5C-DBA565726651}"/>
             <msink:sourceLink direction="with" ref="{73EB1C9E-01B3-4505-9252-C8566026E762}"/>
+            <msink:sourceLink direction="with" ref="{049D7CCE-EC19-40C1-A0C3-5E18631AFB28}"/>
+            <msink:sourceLink direction="with" ref="{0D019606-F597-4B8A-84A9-C7D499D907EF}"/>
             <msink:sourceLink direction="with" ref="{C91A3F93-3FD0-4133-91A3-BA184B45E35A}"/>
-            <msink:sourceLink direction="with" ref="{049D7CCE-EC19-40C1-A0C3-5E18631AFB28}"/>
-            <msink:sourceLink direction="with" ref="{63583EF9-AB05-429F-ACBA-B6DF15FB3804}"/>
-            <msink:sourceLink direction="with" ref="{0D019606-F597-4B8A-84A9-C7D499D907EF}"/>
+            <msink:destinationLink direction="with" ref="{9CE47241-A7D1-4348-AB3B-4D5A32495657}"/>
+            <msink:destinationLink direction="with" ref="{1209F271-C293-45EA-B68C-F6FA2321398B}"/>
+            <msink:destinationLink direction="with" ref="{E66193B9-A86B-4018-A7B8-181B0578DB8B}"/>
             <msink:destinationLink direction="with" ref="{6925F319-5D12-40D7-A878-D8F5676B3FD1}"/>
-            <msink:destinationLink direction="with" ref="{E66193B9-A86B-4018-A7B8-181B0578DB8B}"/>
-            <msink:destinationLink direction="with" ref="{1209F271-C293-45EA-B68C-F6FA2321398B}"/>
-            <msink:destinationLink direction="with" ref="{9CE47241-A7D1-4348-AB3B-4D5A32495657}"/>
             <msink:destinationLink direction="to" ref="{64AAD3BE-0F16-428A-BB30-A1263DC890F6}"/>
           </msink:context>
         </emma:interpretation>
@@ -10986,6 +12183,335 @@
 </inkml:ink>
 </file>
 
+<file path=xl/ink/ink53.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T21:59:08.619"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{961A20EB-0FA6-4A19-9FD7-C9D57C211738}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="21269,775839 23549,774366 23572,774402 21292,775875" semanticType="callout" shapeName="Other">
+            <msink:sourceLink direction="with" ref="{7D32FADB-BC40-400A-8D6B-4EBD2AF762F5}"/>
+            <msink:sourceLink direction="with" ref="{432697DA-EA9F-4883-966A-EFBA6EF87D61}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">10640 388666,'0'0,"0"0,0 0,0 0,0 0,0 0,17-5,5-2,-2-1,13-10,1-4,16-12,7-10,7-7,4-2,0 5,-5 2,0 2,1 2,1 0,4 2,0-1,5-4,3-3,3 5,-1 1,-2-3,1-3,1 3,-3-1,0 1,-3-2,-4 3,-5 1,-1 1,-9 6,-5 3,-6 5,-7-1,-2 1,-1 1,-1 1,-3 3,-4 3,-3 4,-2 5,-3 2,-1 2,-3 0,-1-2,-4 1,2 2,-3-1,1 0,-1 3,-1 0,-3 2,-1 1,-1 1,-1 0,0 0,0 1,0-1</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink54.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T21:59:11.264"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{44A7D587-60E8-47B2-826A-83A95540C1DE}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="24187,777416 26254,775802 26282,775838 24216,777452" semanticType="callout" shapeName="Other">
+            <msink:sourceLink direction="with" ref="{9438EAD1-B2A6-4D36-874B-7EA9E85AB140}"/>
+            <msink:sourceLink direction="with" ref="{B38F42B7-F3F1-4D54-8EF6-26A2524FDF8A}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">14184 387920,'0'0,"0"-1,-19 7,-6 1,1 0,4-2,6-1,6-1,3-2,3 0,2-1,1-1,-13 12,-6 4,2-2,-14 12,-1 1,-10 7,3-2,-8 5,-3 1,2 0,1 3,0-2,-3 0,-4 3,-4 3,-4 5,2 3,-2 0,1 0,0-1,3-1,-2-4,-2-4,-3 0,4 0,2 1,-3 2,-1 3,1 3,7-5,5-6,7-5,5-8,3-1,2-4,0 1,4-1,1-2,2-1,0-1,2-2,1 0,3 0,1-3,1-4,3 1,2-1,3 0,2 0,1-1,0-3,2-1,1-1,2-2,0-1,1 0,0 0,1-1,-1 1,0-1,0 1,0 0,0 0,0 0,0 0</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink55.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T21:59:29.954"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#ED1C24"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{DF0DCBD0-04C9-4099-B1C7-CB2442019791}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="writingRegion" rotatedBoundingBox="22415,774777 22783,774990 22656,775209 22288,774996">
+            <msink:destinationLink direction="with" ref="{855D75B2-841A-41B5-95E2-A843D8E41A26}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{C4EBF4AC-15CF-48DD-89C8-BAC28597517C}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="22415,774777 22783,774990 22656,775209 22288,774996" alignmentLevel="1"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{64D192EF-1163-4F26-8C68-706AA4F422E7}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="line" rotatedBoundingBox="22415,774777 22783,774990 22656,775209 22288,774996"/>
+            </emma:interpretation>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{7D32FADB-BC40-400A-8D6B-4EBD2AF762F5}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="22415,774777 22783,774990 22656,775209 22288,774996">
+                  <msink:destinationLink direction="with" ref="{961A20EB-0FA6-4A19-9FD7-C9D57C211738}"/>
+                  <msink:destinationLink direction="with" ref="{56CA2C78-0A8D-4875-BDD9-53C9E32A978A}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0">11186 387431,'0'-1,"0"1,0 1,0-1,0-1,0 1,0 1,0-1,0-1,0 1,5 17,3 5,-2-2,0 10,-2 0,-2-5,0-7,10 4,2-1,0-4,7-3,1-4,-3-2,3-7,-2-3,0-9,0-9,0-8,-1-3,-4 2,-5 2,-4 7,-2 6,-2 5,-2 5,-1 3,0 1,-3 6,0 6,0 5,-2 6,0 3,2 4,0-1,2-2,4-4,4-2,0-6,1-4,1-4,-1-5,1-4,2-4,0-5,0-2,-1-3,-3 0,-1 2,-3 0,-3 4,-2-1,-1 0,-2 1,-3 3,0 2,-1 3,2 6,1 6,0 0,0 0,2 0,2 1,1-1,1-3,1-1,3-3,1-2,0 0,1-4,1-4,-1 0,-2-3,0-2,-2 0,0-3,-4-1,-1 0,-2 0,-4 2,1 4,-1 4,1 2,2 5,-1 6,-1 5,1 5,-2 5,2-2,2 1,2 0,4-3,2-3,7-1,1-2,2-4,4-6,0-5,-1-6,-2-6,-4-7,-3-2,-3-2,-2-2,-3 3,-2 4,0 2,-2 5,-3 4,-3 4,-4 6,-3 6,-3 7,0 7,0 5,1 2,5-2,4-2,5-5,6-2,6-6,2-2</inkml:trace>
+        </inkml:traceGroup>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink56.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T21:59:35.638"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#ED1C24"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{56CA2C78-0A8D-4875-BDD9-53C9E32A978A}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="22549,774024 22850,777480 22792,777485 22491,774029" semanticType="callout" shapeName="Other">
+            <msink:sourceLink direction="with" ref="{7D32FADB-BC40-400A-8D6B-4EBD2AF762F5}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">11266 387014,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,3 17,0 4,0 0,0 15,-1 1,-1 14,0 11,0 6,-1 6,-1 1,4 6,1 7,2 1,0-1,-1-4,2-2,2 0,3 3,1 4,-1-3,0-6,-2-4,-3-8,1-6,-2-6,1 0,3 3,-2 7,2 3,2 7,0 0,0 5,-4 7,-2 5,-2 3,-2-6,-1-3,1 4,2 8,1 3,1-10,-1-13,-1-14,-2-9,0-8,1 4,1 7,-1 6,-1-9</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink57.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T21:59:33.327"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#ED1C24"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{B5D32BBF-03CB-48C5-B854-95563B70030F}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="writingRegion" rotatedBoundingBox="25633,776479 25383,776666 25187,776405 25436,776218">
+            <msink:destinationLink direction="with" ref="{855D75B2-841A-41B5-95E2-A843D8E41A26}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{F4A20B92-978A-4413-A20A-C931A6B07AD7}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="25633,776479 25383,776666 25187,776405 25436,776218" alignmentLevel="1"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{61251D5D-C7E7-4C81-8A7E-8E0032BA2C74}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="line" rotatedBoundingBox="25633,776479 25383,776666 25187,776405 25436,776218"/>
+            </emma:interpretation>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{9438EAD1-B2A6-4D36-874B-7EA9E85AB140}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="25633,776479 25383,776666 25187,776405 25436,776218">
+                  <msink:destinationLink direction="with" ref="{44A7D587-60E8-47B2-826A-83A95540C1DE}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0">12660 388160,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-3 19,-1 7,1 12,0-1,4 8,1-4,12-1,11-7,10-15,2-14,2-11,-2-12,-2-7,-8-4,-7-1,-8 3,-6 0,-6 3,-6 3,-5 4,-3 6,-6 5,0 4,-4 1,1 6,-2 0,2 4,5-1,4 2,4-1,4-2,6-1,3-2,4-2,3 0,0-1,0-1,0 0,-2 1,-4 0,0-3,-3-1,-4-2,-3-1,-7 2,-1 1,-1 1,-3 5,1 4,1 6,3 10,4 3,3 4,6 1,2 0,5-7,2-6,4-13,2-8,0-7,2-7,-3-3,-3-4,-5 0,-2 5,-5 2,-5 4,-4 6,-1 2,3 4,-2 4,2 8,2 1</inkml:trace>
+        </inkml:traceGroup>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink58.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T21:59:46.921"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#ED1C24"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{855D75B2-841A-41B5-95E2-A843D8E41A26}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="25426,774907 25475,777024 25446,777025 25397,774908" semanticType="verticalRange" shapeName="Line">
+            <msink:sourceLink direction="with" ref="{B5D32BBF-03CB-48C5-B854-95563B70030F}"/>
+            <msink:sourceLink direction="with" ref="{AF354DF0-4BA8-43EC-813C-CB42139B9AB4}"/>
+            <msink:sourceLink direction="with" ref="{DF0DCBD0-04C9-4099-B1C7-CB2442019791}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">12708 387455,'0'0,"0"19,0 7,0-2,0-5,0-5,0-5,0-5,3 12,1 2,-1-2,0 8,-1-1,-1 10,0-1,-1 5,0 4,0 1,0 2,0 0,-1 2,1-1,0-4,0-2,0-3,0-3,0-3,0-2,0 0,0 4,0 1,0 4,0 1,0 1,0 1,0 1,0-4,0-2,0-5,0-2,0-2,0-2,0 0,0 0,0-2,0 0,0-3,0-1,0-1,0 2,0 0,0 3,0 0,3 2,3 3,1 4,0 0,-3 0,0-5,-2-5,-2 0,0-3,0-3,0 2,0-2,0 0,0 1,-1 2,1-2,0-2,0 0,0-2,0-1,0-2,0 0,0 2,0 0,0 0,0 0,0 1,0-1,0-1,0 2,0 0,0 2,0-1,0-1,0-2,0-1,0-1,0 1,0-2,0 2,0-2,0-1,0-2,0 1,0 0,0-2,0 0,0-2,0 0,0-1,0 0,0 0,0 0,0 0,0 0</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink59.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T22:00:05.540"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{432697DA-EA9F-4883-966A-EFBA6EF87D61}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="21358,775854 21811,775854 21811,775869 21358,775869" shapeName="Other">
+            <msink:destinationLink direction="with" ref="{961A20EB-0FA6-4A19-9FD7-C9D57C211738}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">10681 387928,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,0 0,16 0,6 0,-1 0,9 0,0 0,6 0,-4 0,10 0,-3 0,3 0,3 0,7 0,-6 0</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
 <file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
@@ -11018,6 +12544,218 @@
       </emma:emma>
     </inkml:annotationXML>
     <inkml:trace contextRef="#ctx0" brushRef="#br0">11230 93761,'0'0,"0"0,0 0,0 0,9-2,2 0,13 0,9 1,7 0,8 0,6 1,6 0,4 0,6 0,4 0,6 0,5 0,6 0,1 0,4 0,1 0,-2 0,-3 2,-4-1,-6 1,-6 0,0 2,3 2,-2 1,2 1,5 1,5-1,5 0,3-2,4 0,2 0,0-2,-3-1,-6-1,-3-1,-2-1,-1 0,0 0,-4 0,1-4,-1 0,-1 1,-2 0,-3 1,-4-1,-4 0,0 1,0 1,-3 0,0-1,-1 0,0-1,0 0,-2-1,-6 0,0 0,-1 1,-2-2,-3 1,1-1,0-1,3-1,0 0,-2 1,-2-1,-2 0,0 1,1 0,-2 1,-1 0,-2 0,-2 1,0-1,0 1,-2 0,0 2,-2 0,2-1,-2 1,2 1,-1 0,1 0,0 0,0-1,0 0,1 1,3 0,0 0,-1 1,-4 0,-3 0,-6 0,-5 0,-6 0,-5 0,-5 0,-4 0,-3-1,-2-1</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink60.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T22:00:07.324"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{5ABED61C-F9E9-463E-AC6C-6373B8902200}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="writingRegion" rotatedBoundingBox="25464,775822 26491,775822 26491,775839 25464,775839"/>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{B8856C4C-1394-4F28-AA87-24F2522B1A07}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="25464,775822 26491,775822 26491,775839 25464,775839" alignmentLevel="1"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{99E972BF-8A46-4D82-95F6-1918D2DF3F3E}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="line" rotatedBoundingBox="25464,775822 26491,775822 26491,775839 25464,775839"/>
+            </emma:interpretation>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{25BC0517-41A1-4CBE-B359-A0797E8BED34}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="25464,775838 25693,775838 25693,775839 25464,775839"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0">12732 387920,'0'0,"0"-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,19 0,7 0,-2 0,9 0,-1 0,5 0,-4 0,-8 0</inkml:trace>
+        </inkml:traceGroup>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{B38F42B7-F3F1-4D54-8EF6-26A2524FDF8A}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="26249,775822 26491,775822 26491,775838 26249,775838">
+                  <msink:destinationLink direction="with" ref="{44A7D587-60E8-47B2-826A-83A95540C1DE}"/>
+                </msink:context>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="390">13517 387919,'0'0,"0"0,0 0,0 0,0 0,0 0,0 0,19-3,7 0,-2 0,12 0,0 1,15 1,-1 0</inkml:trace>
+        </inkml:traceGroup>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink61.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T22:00:06.941"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{AF354DF0-4BA8-43EC-813C-CB42139B9AB4}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="writingRegion" rotatedBoundingBox="24405,775774 24714,775774 24714,775789 24405,775789">
+            <msink:destinationLink direction="with" ref="{855D75B2-841A-41B5-95E2-A843D8E41A26}"/>
+          </msink:context>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:traceGroup>
+      <inkml:annotationXML>
+        <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+          <emma:interpretation id="{E3F05720-F1E9-4740-AE0A-9F25872892CE}" emma:medium="tactile" emma:mode="ink">
+            <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="paragraph" rotatedBoundingBox="24405,775774 24714,775774 24714,775789 24405,775789" alignmentLevel="1"/>
+          </emma:interpretation>
+        </emma:emma>
+      </inkml:annotationXML>
+      <inkml:traceGroup>
+        <inkml:annotationXML>
+          <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+            <emma:interpretation id="{9E314C22-816D-4C33-A4A8-7CB623AE513F}" emma:medium="tactile" emma:mode="ink">
+              <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="line" rotatedBoundingBox="24405,775774 24714,775774 24714,775789 24405,775789"/>
+            </emma:interpretation>
+          </emma:emma>
+        </inkml:annotationXML>
+        <inkml:traceGroup>
+          <inkml:annotationXML>
+            <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+              <emma:interpretation id="{FB16B42D-2258-41E8-BB66-9118608E1BDE}" emma:medium="tactile" emma:mode="ink">
+                <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkWord" rotatedBoundingBox="24405,775774 24714,775774 24714,775789 24405,775789"/>
+              </emma:interpretation>
+            </emma:emma>
+          </inkml:annotationXML>
+          <inkml:trace contextRef="#ctx0" brushRef="#br0">12204 387888,'0'0,"0"0,0 0,0 0,0 0,0 0,16 0,6 0,-1 0,-5 0,-3 0,-6 0,13 0,3 0,-1 0,7 0,0 0,6 0,-3 0,-8 0</inkml:trace>
+        </inkml:traceGroup>
+      </inkml:traceGroup>
+    </inkml:traceGroup>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink62.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T22:00:06.566"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{9A732DFE-3A4E-4F12-9537-DBCAE837C4F9}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="23490,775838 23953,775837 23954,775838 23491,775839" shapeName="Other"/>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">11747 387920,'16'0,"6"-1,-1 1,-5 0,-4 0,-4 0,-4 0,-3 0,-1 0,13 0,4 0,10 0,1 0,6 0,-2 0,4 0,-4 0,3 0,2 0,1 0,-4 0</inkml:trace>
+  </inkml:traceGroup>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink63.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2017-01-10T22:00:06.054"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="height" value="0.02333" units="cm"/>
+      <inkml:brushProperty name="color" value="#3165BB"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:traceGroup>
+    <inkml:annotationXML>
+      <emma:emma xmlns:emma="http://www.w3.org/2003/04/emma" version="1.0">
+        <emma:interpretation id="{7784F3DB-80CB-4287-BE26-32BD1BA83FF2}" emma:medium="tactile" emma:mode="ink">
+          <msink:context xmlns:msink="http://schemas.microsoft.com/ink/2010/main" type="inkDrawing" rotatedBoundingBox="22416,775869 22973,775853 22973,775862 22417,775878" shapeName="Other"/>
+        </emma:interpretation>
+      </emma:emma>
+    </inkml:annotationXML>
+    <inkml:trace contextRef="#ctx0" brushRef="#br0">11209 387944,'0'0,"0"0,19 0,7 0,-2 0,-5 0,-5 0,-5 0,-5 0,-2 0,-2 0,0 0,15 0,6 0,12 0,1 0,6 0,4 0,2-2,0-2,0 0,-3 1,-3 1,-9 1</inkml:trace>
   </inkml:traceGroup>
 </inkml:ink>
 </file>
@@ -11626,19 +13364,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH190"/>
+  <dimension ref="A1:AH203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E187" sqref="E187"/>
+      <selection pane="bottomLeft" activeCell="H196" sqref="H196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.54296875" style="8" customWidth="1"/>
     <col min="2" max="2" width="4.1796875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="56.6328125" style="22" customWidth="1"/>
     <col min="5" max="5" width="60.36328125" style="12" customWidth="1"/>
     <col min="7" max="7" width="11.36328125" style="8" customWidth="1"/>
@@ -11729,7 +13467,7 @@
         <v>71</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="AB1" s="3" t="s">
         <v>105</v>
@@ -11747,10 +13485,10 @@
         <v>373</v>
       </c>
       <c r="AG1" s="7" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="AH1" s="24" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -13995,7 +15733,7 @@
       <c r="B50" s="2">
         <v>24</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="2" t="s">
         <v>151</v>
       </c>
       <c r="E50" s="13" t="s">
@@ -14021,7 +15759,7 @@
       <c r="B51" s="2">
         <v>345</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="2" t="s">
         <v>153</v>
       </c>
       <c r="E51" s="13" t="s">
@@ -14050,7 +15788,7 @@
       <c r="B52" s="2">
         <v>125</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="2" t="s">
         <v>155</v>
       </c>
       <c r="E52" s="13" t="s">
@@ -14076,7 +15814,7 @@
       <c r="B53" s="2">
         <v>28</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="2" t="s">
         <v>157</v>
       </c>
       <c r="E53" s="13" t="s">
@@ -14102,7 +15840,7 @@
       <c r="B54" s="2">
         <v>223</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="2" t="s">
         <v>159</v>
       </c>
       <c r="D54" s="22" t="s">
@@ -14125,7 +15863,7 @@
       <c r="B55" s="2">
         <v>66</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="2" t="s">
         <v>161</v>
       </c>
       <c r="D55" s="22" t="s">
@@ -14148,7 +15886,7 @@
       <c r="B56" s="2">
         <v>112</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="2" t="s">
         <v>162</v>
       </c>
       <c r="D56" s="22" t="s">
@@ -14180,7 +15918,7 @@
       <c r="B57" s="2">
         <v>113</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="2" t="s">
         <v>166</v>
       </c>
       <c r="D57" s="22" t="s">
@@ -14215,7 +15953,7 @@
       <c r="B58" s="2">
         <v>205</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="2" t="s">
         <v>170</v>
       </c>
       <c r="D58" s="22" t="s">
@@ -14244,7 +15982,7 @@
       <c r="B59" s="8">
         <v>290</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="2" t="s">
         <v>172</v>
       </c>
       <c r="E59" s="16" t="s">
@@ -14299,7 +16037,7 @@
       <c r="B61" s="2">
         <v>278</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="2" t="s">
         <v>177</v>
       </c>
       <c r="E61" s="13" t="s">
@@ -14325,7 +16063,7 @@
       <c r="B62" s="2">
         <v>36</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="2" t="s">
         <v>180</v>
       </c>
       <c r="E62" s="13" t="s">
@@ -14351,7 +16089,7 @@
       <c r="B63" s="2">
         <v>219</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="2" t="s">
         <v>181</v>
       </c>
       <c r="F63" s="2" t="s">
@@ -14374,7 +16112,7 @@
       <c r="B64" s="2">
         <v>220</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="2" t="s">
         <v>183</v>
       </c>
       <c r="E64" s="13" t="s">
@@ -14394,7 +16132,7 @@
       <c r="B65" s="2">
         <v>38</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="2" t="s">
         <v>185</v>
       </c>
       <c r="D65" s="22" t="s">
@@ -14414,7 +16152,7 @@
       <c r="B66" s="2">
         <v>58</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E66" s="13" t="s">
@@ -14434,7 +16172,7 @@
       <c r="B67" s="2">
         <v>14</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="2" t="s">
         <v>189</v>
       </c>
       <c r="F67" s="2" t="s">
@@ -14454,7 +16192,7 @@
       <c r="B68" s="2">
         <v>198</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="2" t="s">
         <v>190</v>
       </c>
       <c r="D68" s="22" t="s">
@@ -14476,14 +16214,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:29" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B69" s="2">
         <v>303</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="2" t="s">
         <v>193</v>
       </c>
       <c r="E69" s="12" t="s">
@@ -14509,7 +16247,7 @@
       <c r="B70" s="2">
         <v>121</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="2" t="s">
         <v>196</v>
       </c>
       <c r="E70" s="13" t="s">
@@ -14532,7 +16270,7 @@
       <c r="B71" s="2">
         <v>70</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="2" t="s">
         <v>199</v>
       </c>
       <c r="D71" s="22" t="s">
@@ -14561,7 +16299,7 @@
       <c r="B72" s="2">
         <v>67</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="2" t="s">
         <v>202</v>
       </c>
       <c r="E72" s="13" t="s">
@@ -14587,7 +16325,7 @@
       <c r="B73" s="2">
         <v>396</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="2" t="s">
         <v>204</v>
       </c>
       <c r="F73" s="2" t="s">
@@ -14610,7 +16348,7 @@
       <c r="B74" s="2">
         <v>155</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="2" t="s">
         <v>205</v>
       </c>
       <c r="D74" s="22" t="s">
@@ -14659,7 +16397,7 @@
       <c r="B76" s="2">
         <v>414</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="2" t="s">
         <v>210</v>
       </c>
       <c r="E76" s="12" t="s">
@@ -14682,7 +16420,7 @@
       <c r="B77" s="2">
         <v>240</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="2" t="s">
         <v>212</v>
       </c>
       <c r="D77" s="22" t="s">
@@ -14708,7 +16446,7 @@
       <c r="B78" s="2">
         <v>35</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C78" s="2" t="s">
         <v>217</v>
       </c>
       <c r="E78" s="12" t="s">
@@ -14754,7 +16492,7 @@
       <c r="B80" s="2">
         <v>74</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="2" t="s">
         <v>221</v>
       </c>
       <c r="D80" s="22" t="s">
@@ -14844,7 +16582,7 @@
       <c r="B83" s="2">
         <v>189</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" s="2" t="s">
         <v>229</v>
       </c>
       <c r="D83" s="22" t="s">
@@ -14873,7 +16611,7 @@
       <c r="B84" s="2">
         <v>61</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C84" s="2" t="s">
         <v>232</v>
       </c>
       <c r="D84" s="22" t="s">
@@ -14948,7 +16686,7 @@
       <c r="B87" s="2">
         <v>165</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E87" s="13" t="s">
@@ -14971,7 +16709,7 @@
       <c r="B88" s="2">
         <v>338</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="2" t="s">
         <v>242</v>
       </c>
       <c r="E88" s="13" t="s">
@@ -14997,7 +16735,7 @@
       <c r="B89" s="2">
         <v>319</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="2" t="s">
         <v>245</v>
       </c>
       <c r="D89" s="22" t="s">
@@ -15023,7 +16761,7 @@
       <c r="B90" s="2">
         <v>268</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" s="2" t="s">
         <v>244</v>
       </c>
       <c r="D90" s="22" t="s">
@@ -15107,7 +16845,7 @@
       <c r="B93" s="2">
         <v>347</v>
       </c>
-      <c r="C93" s="8" t="s">
+      <c r="C93" s="2" t="s">
         <v>258</v>
       </c>
       <c r="D93" s="22" t="s">
@@ -15126,14 +16864,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:31" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B94" s="2">
         <v>215</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C94" s="2" t="s">
         <v>261</v>
       </c>
       <c r="F94" s="2" t="s">
@@ -15156,7 +16894,7 @@
       <c r="B95" s="2">
         <v>75</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C95" s="2" t="s">
         <v>262</v>
       </c>
       <c r="D95" s="22" t="s">
@@ -15185,7 +16923,7 @@
       <c r="B96" s="2">
         <v>22</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C96" s="2" t="s">
         <v>268</v>
       </c>
       <c r="E96" s="13" t="s">
@@ -15208,7 +16946,7 @@
       <c r="B97" s="2">
         <v>39</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="2" t="s">
         <v>269</v>
       </c>
       <c r="F97" s="2" t="s">
@@ -15228,7 +16966,7 @@
       <c r="B98" s="2">
         <v>40</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C98" s="2" t="s">
         <v>271</v>
       </c>
       <c r="E98" s="13" t="s">
@@ -15251,7 +16989,7 @@
       <c r="B99" s="2">
         <v>46</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="2" t="s">
         <v>273</v>
       </c>
       <c r="E99" s="12" t="s">
@@ -15274,7 +17012,7 @@
       <c r="B100" s="2">
         <v>47</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C100" s="2" t="s">
         <v>275</v>
       </c>
       <c r="E100" s="12" t="s">
@@ -15297,7 +17035,7 @@
       <c r="B101" s="2">
         <v>92</v>
       </c>
-      <c r="C101" s="8" t="s">
+      <c r="C101" s="2" t="s">
         <v>277</v>
       </c>
       <c r="D101" s="22" t="s">
@@ -15323,7 +17061,7 @@
       <c r="B102" s="2">
         <v>339</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C102" s="2" t="s">
         <v>283</v>
       </c>
       <c r="D102" s="22" t="s">
@@ -15358,7 +17096,7 @@
       <c r="B103" s="2">
         <v>252</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="2" t="s">
         <v>285</v>
       </c>
       <c r="D103" s="22" t="s">
@@ -15393,7 +17131,7 @@
       <c r="B104" s="2">
         <v>266</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C104" s="2" t="s">
         <v>293</v>
       </c>
       <c r="D104" s="22" t="s">
@@ -15422,7 +17160,7 @@
       <c r="B105" s="2">
         <v>243</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="2" t="s">
         <v>297</v>
       </c>
       <c r="D105" s="22" t="s">
@@ -15451,7 +17189,7 @@
       <c r="B106" s="2">
         <v>246</v>
       </c>
-      <c r="C106" s="8" t="s">
+      <c r="C106" s="2" t="s">
         <v>299</v>
       </c>
       <c r="D106" s="22" t="s">
@@ -15480,7 +17218,7 @@
       <c r="B107" s="2">
         <v>276</v>
       </c>
-      <c r="C107" s="8" t="s">
+      <c r="C107" s="2" t="s">
         <v>300</v>
       </c>
       <c r="D107" s="22" t="s">
@@ -15512,7 +17250,7 @@
       <c r="B108" s="2">
         <v>270</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="C108" s="2" t="s">
         <v>304</v>
       </c>
       <c r="D108" s="22" t="s">
@@ -15547,7 +17285,7 @@
       <c r="B109" s="2">
         <v>170</v>
       </c>
-      <c r="C109" s="8" t="s">
+      <c r="C109" s="2" t="s">
         <v>306</v>
       </c>
       <c r="D109" s="22" t="s">
@@ -15573,7 +17311,7 @@
       <c r="B110" s="2">
         <v>167</v>
       </c>
-      <c r="C110" s="8" t="s">
+      <c r="C110" s="2" t="s">
         <v>316</v>
       </c>
       <c r="D110" s="22" t="s">
@@ -15608,7 +17346,7 @@
       <c r="B111" s="2">
         <v>280</v>
       </c>
-      <c r="C111" s="8" t="s">
+      <c r="C111" s="2" t="s">
         <v>320</v>
       </c>
       <c r="D111" s="22" t="s">
@@ -15643,7 +17381,7 @@
       <c r="B112" s="2">
         <v>366</v>
       </c>
-      <c r="C112" s="8" t="s">
+      <c r="C112" s="2" t="s">
         <v>327</v>
       </c>
       <c r="D112" s="22" t="s">
@@ -15678,7 +17416,7 @@
       <c r="B113" s="2">
         <v>364</v>
       </c>
-      <c r="C113" s="8" t="s">
+      <c r="C113" s="2" t="s">
         <v>328</v>
       </c>
       <c r="D113" s="22" t="s">
@@ -15710,7 +17448,7 @@
       <c r="B114" s="2">
         <v>249</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="C114" s="2" t="s">
         <v>330</v>
       </c>
       <c r="D114" s="22" t="s">
@@ -15742,7 +17480,7 @@
       <c r="B115" s="2">
         <v>320</v>
       </c>
-      <c r="C115" s="8" t="s">
+      <c r="C115" s="2" t="s">
         <v>335</v>
       </c>
       <c r="D115" s="22" t="s">
@@ -15774,7 +17512,7 @@
       <c r="B116" s="2">
         <v>254</v>
       </c>
-      <c r="C116" s="8" t="s">
+      <c r="C116" s="2" t="s">
         <v>338</v>
       </c>
       <c r="D116" s="22" t="s">
@@ -15809,7 +17547,7 @@
       <c r="B117" s="2">
         <v>131</v>
       </c>
-      <c r="C117" s="8" t="s">
+      <c r="C117" s="2" t="s">
         <v>343</v>
       </c>
       <c r="D117" s="22" t="s">
@@ -15844,7 +17582,7 @@
       <c r="B118" s="2">
         <v>89</v>
       </c>
-      <c r="C118" s="8" t="s">
+      <c r="C118" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D118" s="22" t="s">
@@ -15873,7 +17611,7 @@
       <c r="B119" s="2">
         <v>77</v>
       </c>
-      <c r="C119" s="8" t="s">
+      <c r="C119" s="2" t="s">
         <v>350</v>
       </c>
       <c r="D119" s="22" t="s">
@@ -15899,7 +17637,7 @@
       <c r="B120" s="2">
         <v>216</v>
       </c>
-      <c r="C120" s="8" t="s">
+      <c r="C120" s="2" t="s">
         <v>351</v>
       </c>
       <c r="D120" s="22" t="s">
@@ -15928,7 +17666,7 @@
       <c r="B121" s="2">
         <v>60</v>
       </c>
-      <c r="C121" s="8" t="s">
+      <c r="C121" s="2" t="s">
         <v>355</v>
       </c>
       <c r="D121" s="22" t="s">
@@ -15989,7 +17727,7 @@
       <c r="B123" s="2">
         <v>79</v>
       </c>
-      <c r="C123" s="8" t="s">
+      <c r="C123" s="2" t="s">
         <v>365</v>
       </c>
       <c r="D123" s="22" t="s">
@@ -16088,11 +17826,11 @@
       <c r="B126" s="2">
         <v>288</v>
       </c>
-      <c r="C126" s="8" t="s">
+      <c r="C126" s="2" t="s">
         <v>377</v>
       </c>
       <c r="D126" s="22" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E126" s="13" t="s">
         <v>376</v>
@@ -16123,7 +17861,7 @@
       <c r="B127" s="2">
         <v>392</v>
       </c>
-      <c r="C127" s="8" t="s">
+      <c r="C127" s="2" t="s">
         <v>379</v>
       </c>
       <c r="D127" s="22" t="s">
@@ -16152,7 +17890,7 @@
       <c r="B128" s="2">
         <v>153</v>
       </c>
-      <c r="C128" s="8" t="s">
+      <c r="C128" s="2" t="s">
         <v>382</v>
       </c>
       <c r="D128" s="22" t="s">
@@ -16184,7 +17922,7 @@
       <c r="B129" s="2">
         <v>274</v>
       </c>
-      <c r="C129" s="8" t="s">
+      <c r="C129" s="2" t="s">
         <v>386</v>
       </c>
       <c r="D129" s="22" t="s">
@@ -16216,7 +17954,7 @@
       <c r="B130" s="2">
         <v>275</v>
       </c>
-      <c r="C130" s="8" t="s">
+      <c r="C130" s="2" t="s">
         <v>389</v>
       </c>
       <c r="D130" s="22" t="s">
@@ -16248,7 +17986,7 @@
       <c r="B131" s="2">
         <v>475</v>
       </c>
-      <c r="C131" s="8" t="s">
+      <c r="C131" s="2" t="s">
         <v>393</v>
       </c>
       <c r="D131" s="22" t="s">
@@ -16280,7 +18018,7 @@
       <c r="B132" s="2">
         <v>50</v>
       </c>
-      <c r="C132" s="8" t="s">
+      <c r="C132" s="2" t="s">
         <v>398</v>
       </c>
       <c r="D132" s="22" t="s">
@@ -16345,7 +18083,7 @@
         <v>405</v>
       </c>
       <c r="E134" s="13" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>314</v>
@@ -16367,7 +18105,7 @@
       <c r="B135" s="2">
         <v>292</v>
       </c>
-      <c r="C135" s="8" t="s">
+      <c r="C135" s="2" t="s">
         <v>406</v>
       </c>
       <c r="D135" s="22" t="s">
@@ -16399,7 +18137,7 @@
       <c r="B136" s="2">
         <v>409</v>
       </c>
-      <c r="C136" s="8" t="s">
+      <c r="C136" s="2" t="s">
         <v>410</v>
       </c>
       <c r="D136" s="22" t="s">
@@ -16428,7 +18166,7 @@
       <c r="B137" s="2">
         <v>401</v>
       </c>
-      <c r="C137" s="8" t="s">
+      <c r="C137" s="2" t="s">
         <v>415</v>
       </c>
       <c r="D137" s="22" t="s">
@@ -16457,7 +18195,7 @@
       <c r="B138" s="2">
         <v>293</v>
       </c>
-      <c r="C138" s="8" t="s">
+      <c r="C138" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D138" s="22" t="s">
@@ -16483,7 +18221,7 @@
       <c r="B139" s="2">
         <v>294</v>
       </c>
-      <c r="C139" s="8" t="s">
+      <c r="C139" s="2" t="s">
         <v>420</v>
       </c>
       <c r="D139" s="22" t="s">
@@ -16512,14 +18250,14 @@
       <c r="B140" s="2">
         <v>464</v>
       </c>
-      <c r="C140" s="8" t="s">
+      <c r="C140" s="2" t="s">
         <v>423</v>
       </c>
       <c r="D140" s="22" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E140" s="13" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>81</v>
@@ -16548,16 +18286,16 @@
         <v>46</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D141" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E141" s="13" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>81</v>
@@ -16579,11 +18317,11 @@
       <c r="B142" s="2">
         <v>412</v>
       </c>
-      <c r="C142" s="8" t="s">
-        <v>442</v>
+      <c r="C142" s="2" t="s">
+        <v>439</v>
       </c>
       <c r="D142" s="22" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>32</v>
@@ -16599,14 +18337,14 @@
       <c r="B143" s="2">
         <v>415</v>
       </c>
-      <c r="C143" s="8" t="s">
-        <v>445</v>
+      <c r="C143" s="2" t="s">
+        <v>442</v>
       </c>
       <c r="D143" s="22" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E143" s="13" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>32</v>
@@ -16615,7 +18353,7 @@
         <v>42728</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="144" spans="1:30" ht="217.5" x14ac:dyDescent="0.35">
@@ -16625,17 +18363,17 @@
       <c r="B144" s="2">
         <v>437</v>
       </c>
-      <c r="C144" s="8" t="s">
-        <v>451</v>
+      <c r="C144" s="2" t="s">
+        <v>448</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E144" s="13" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G144" s="9">
         <v>42728</v>
@@ -16664,13 +18402,13 @@
         <v>300</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D145" s="22" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="E145" s="13" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>81</v>
@@ -16698,14 +18436,14 @@
       <c r="B146" s="2">
         <v>354</v>
       </c>
-      <c r="C146" s="8" t="s">
+      <c r="C146" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D146" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="E146" s="13" t="s">
         <v>462</v>
-      </c>
-      <c r="D146" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="E146" s="13" t="s">
-        <v>465</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>81</v>
@@ -16734,13 +18472,13 @@
         <v>406</v>
       </c>
       <c r="C147" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D147" s="22" t="s">
+        <v>458</v>
+      </c>
+      <c r="E147" s="13" t="s">
         <v>457</v>
-      </c>
-      <c r="D147" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="E147" s="13" t="s">
-        <v>460</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>81</v>
@@ -16762,14 +18500,14 @@
       <c r="B148" s="2">
         <v>434</v>
       </c>
-      <c r="C148" s="8" t="s">
+      <c r="C148" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D148" s="22" t="s">
         <v>463</v>
       </c>
-      <c r="D148" s="22" t="s">
-        <v>466</v>
-      </c>
       <c r="E148" s="13" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>69</v>
@@ -16788,14 +18526,14 @@
       <c r="B149" s="2">
         <v>15</v>
       </c>
-      <c r="C149" s="8" t="s">
-        <v>467</v>
+      <c r="C149" s="2" t="s">
+        <v>464</v>
       </c>
       <c r="D149" s="22" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E149" s="13" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>69</v>
@@ -16804,7 +18542,7 @@
         <v>42732</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="150" spans="1:33" ht="261" x14ac:dyDescent="0.35">
@@ -16814,17 +18552,17 @@
       <c r="B150" s="2">
         <v>18</v>
       </c>
-      <c r="C150" s="8" t="s">
+      <c r="C150" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="D150" s="22" t="s">
         <v>470</v>
       </c>
-      <c r="D150" s="22" t="s">
-        <v>473</v>
-      </c>
       <c r="E150" s="13" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G150" s="9">
         <v>42733</v>
@@ -16840,14 +18578,14 @@
       <c r="B151" s="2">
         <v>16</v>
       </c>
-      <c r="C151" s="8" t="s">
-        <v>475</v>
+      <c r="C151" s="2" t="s">
+        <v>472</v>
       </c>
       <c r="D151" s="22" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E151" s="13" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>69</v>
@@ -16872,14 +18610,14 @@
       <c r="B152" s="2">
         <v>259</v>
       </c>
-      <c r="C152" s="8" t="s">
-        <v>478</v>
+      <c r="C152" s="2" t="s">
+        <v>475</v>
       </c>
       <c r="D152" s="22" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E152" s="13" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>4</v>
@@ -16910,14 +18648,14 @@
       <c r="B153" s="2">
         <v>454</v>
       </c>
-      <c r="C153" s="8" t="s">
+      <c r="C153" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="D153" s="22" t="s">
         <v>481</v>
       </c>
-      <c r="D153" s="22" t="s">
-        <v>484</v>
-      </c>
       <c r="E153" s="13" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>81</v>
@@ -16937,13 +18675,13 @@
         <v>453</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D154" s="22" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E154" s="13" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>59</v>
@@ -16952,7 +18690,7 @@
         <v>42734</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="S154" s="8" t="s">
         <v>5</v>
@@ -16966,13 +18704,13 @@
         <v>462</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D155" s="22" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E155" s="13" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F155" s="2" t="s">
         <v>69</v>
@@ -16991,11 +18729,11 @@
       <c r="B156" s="2">
         <v>86</v>
       </c>
-      <c r="C156" s="8" t="s">
-        <v>493</v>
+      <c r="C156" s="2" t="s">
+        <v>490</v>
       </c>
       <c r="D156" s="22" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F156" s="2" t="s">
         <v>59</v>
@@ -17017,11 +18755,11 @@
       <c r="B157" s="2">
         <v>142</v>
       </c>
-      <c r="C157" s="8" t="s">
-        <v>497</v>
+      <c r="C157" s="2" t="s">
+        <v>494</v>
       </c>
       <c r="D157" s="22" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>81</v>
@@ -17050,13 +18788,13 @@
         <v>109</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D158" s="22" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E158" s="13" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>59</v>
@@ -17065,7 +18803,7 @@
         <v>42736</v>
       </c>
       <c r="H158" s="8" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="K158" s="8" t="s">
         <v>5</v>
@@ -17085,13 +18823,13 @@
         <v>108</v>
       </c>
       <c r="C159" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="D159" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="E159" s="19" t="s">
         <v>499</v>
-      </c>
-      <c r="D159" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="E159" s="19" t="s">
-        <v>502</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>32</v>
@@ -17100,7 +18838,7 @@
         <v>42736</v>
       </c>
       <c r="H159" s="8" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="N159" s="8" t="s">
         <v>5</v>
@@ -17116,14 +18854,14 @@
       <c r="B160" s="2">
         <v>82</v>
       </c>
-      <c r="C160" s="8" t="s">
-        <v>504</v>
+      <c r="C160" s="2" t="s">
+        <v>501</v>
       </c>
       <c r="D160" s="22" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E160" s="13" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>69</v>
@@ -17139,14 +18877,14 @@
       <c r="B161" s="2">
         <v>2</v>
       </c>
-      <c r="C161" s="8" t="s">
+      <c r="C161" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D161" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="E161" s="13" t="s">
         <v>506</v>
-      </c>
-      <c r="D161" s="22" t="s">
-        <v>508</v>
-      </c>
-      <c r="E161" s="13" t="s">
-        <v>509</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>59</v>
@@ -17155,7 +18893,7 @@
         <v>42736</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="N161" s="8" t="s">
         <v>5</v>
@@ -17168,14 +18906,14 @@
       <c r="B162" s="2">
         <v>445</v>
       </c>
-      <c r="C162" s="8" t="s">
+      <c r="C162" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="D162" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="E162" s="12" t="s">
         <v>510</v>
-      </c>
-      <c r="D162" s="22" t="s">
-        <v>511</v>
-      </c>
-      <c r="E162" s="12" t="s">
-        <v>513</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>81</v>
@@ -17184,7 +18922,7 @@
         <v>42736</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="N162" s="8" t="s">
         <v>5</v>
@@ -17203,14 +18941,14 @@
       <c r="B163" s="2">
         <v>43</v>
       </c>
-      <c r="C163" s="8" t="s">
+      <c r="C163" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="D163" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="E163" s="20" t="s">
         <v>514</v>
-      </c>
-      <c r="D163" s="22" t="s">
-        <v>515</v>
-      </c>
-      <c r="E163" s="20" t="s">
-        <v>517</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>4</v>
@@ -17219,7 +18957,7 @@
         <v>42737</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="O163" s="8" t="s">
         <v>5</v>
@@ -17235,14 +18973,14 @@
       <c r="B164" s="2">
         <v>418</v>
       </c>
-      <c r="C164" s="8" t="s">
-        <v>519</v>
+      <c r="C164" s="2" t="s">
+        <v>516</v>
       </c>
       <c r="D164" s="22" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E164" s="13" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F164" s="2" t="s">
         <v>4</v>
@@ -17264,14 +19002,14 @@
       <c r="B165" s="2">
         <v>53</v>
       </c>
-      <c r="C165" s="8" t="s">
-        <v>523</v>
+      <c r="C165" s="2" t="s">
+        <v>520</v>
       </c>
       <c r="D165" s="22" t="s">
+        <v>518</v>
+      </c>
+      <c r="E165" s="13" t="s">
         <v>521</v>
-      </c>
-      <c r="E165" s="13" t="s">
-        <v>524</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>32</v>
@@ -17280,7 +19018,7 @@
         <v>42740</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="L165" s="8" t="s">
         <v>5</v>
@@ -17299,14 +19037,14 @@
       <c r="B166" s="2">
         <v>152</v>
       </c>
-      <c r="C166" s="8" t="s">
-        <v>525</v>
+      <c r="C166" s="2" t="s">
+        <v>522</v>
       </c>
       <c r="D166" s="22" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E166" s="13" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>59</v>
@@ -17331,14 +19069,14 @@
       <c r="B167" s="2">
         <v>343</v>
       </c>
-      <c r="C167" s="8" t="s">
-        <v>528</v>
+      <c r="C167" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="D167" s="22" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E167" s="13" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>81</v>
@@ -17357,14 +19095,14 @@
       <c r="B168" s="2">
         <v>139</v>
       </c>
-      <c r="C168" s="8" t="s">
-        <v>533</v>
+      <c r="C168" s="2" t="s">
+        <v>530</v>
       </c>
       <c r="D168" s="22" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E168" s="17" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>81</v>
@@ -17373,7 +19111,7 @@
         <v>42741</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="O168" s="8" t="s">
         <v>5</v>
@@ -17389,14 +19127,14 @@
       <c r="B169" s="2">
         <v>279</v>
       </c>
-      <c r="C169" s="8" t="s">
-        <v>540</v>
+      <c r="C169" s="2" t="s">
+        <v>537</v>
       </c>
       <c r="D169" s="22" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E169" s="13" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>81</v>
@@ -17424,14 +19162,14 @@
       <c r="B170" s="2">
         <v>120</v>
       </c>
-      <c r="C170" s="8" t="s">
-        <v>542</v>
+      <c r="C170" s="2" t="s">
+        <v>539</v>
       </c>
       <c r="D170" s="22" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E170" s="13" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>32</v>
@@ -17453,14 +19191,14 @@
       <c r="B171" s="2">
         <v>62</v>
       </c>
-      <c r="C171" s="8" t="s">
-        <v>546</v>
+      <c r="C171" s="2" t="s">
+        <v>543</v>
       </c>
       <c r="D171" s="23" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E171" s="17" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>69</v>
@@ -17485,14 +19223,14 @@
       <c r="B172" s="2">
         <v>63</v>
       </c>
-      <c r="C172" s="8" t="s">
-        <v>548</v>
+      <c r="C172" s="2" t="s">
+        <v>545</v>
       </c>
       <c r="D172" s="22" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E172" s="13" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="F172" s="2" t="s">
         <v>32</v>
@@ -17517,14 +19255,14 @@
       <c r="B173" s="2">
         <v>64</v>
       </c>
-      <c r="C173" s="8" t="s">
-        <v>551</v>
+      <c r="C173" s="2" t="s">
+        <v>548</v>
       </c>
       <c r="D173" s="22" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E173" s="12" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>32</v>
@@ -17546,14 +19284,14 @@
       <c r="B174" s="2">
         <v>264</v>
       </c>
-      <c r="C174" s="8" t="s">
-        <v>554</v>
+      <c r="C174" s="2" t="s">
+        <v>551</v>
       </c>
       <c r="D174" s="21" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E174" s="13" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F174" s="2" t="s">
         <v>81</v>
@@ -17573,10 +19311,10 @@
         <v>47</v>
       </c>
       <c r="D175" s="22" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E175" s="13" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F175" s="2" t="s">
         <v>32</v>
@@ -17616,14 +19354,14 @@
       <c r="B176" s="8">
         <v>23</v>
       </c>
-      <c r="C176" s="8" t="s">
-        <v>563</v>
+      <c r="C176" s="2" t="s">
+        <v>560</v>
       </c>
       <c r="D176" s="21" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E176" s="13" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="F176" s="2" t="s">
         <v>32</v>
@@ -17632,7 +19370,7 @@
         <v>42742</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="N176" s="8" t="s">
         <v>5</v>
@@ -17651,14 +19389,14 @@
       <c r="B177" s="8">
         <v>95</v>
       </c>
-      <c r="C177" s="8" t="s">
-        <v>566</v>
+      <c r="C177" s="2" t="s">
+        <v>563</v>
       </c>
       <c r="D177" s="21" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E177" s="13" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>81</v>
@@ -17683,14 +19421,14 @@
       <c r="B178" s="8">
         <v>376</v>
       </c>
-      <c r="C178" s="8" t="s">
-        <v>570</v>
+      <c r="C178" s="2" t="s">
+        <v>567</v>
       </c>
       <c r="D178" s="22" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E178" s="13" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F178" s="2" t="s">
         <v>32</v>
@@ -17712,14 +19450,14 @@
       <c r="B179" s="8">
         <v>204</v>
       </c>
-      <c r="C179" s="8" t="s">
-        <v>572</v>
+      <c r="C179" s="2" t="s">
+        <v>569</v>
       </c>
       <c r="D179" s="22" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E179" s="13" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>81</v>
@@ -17738,14 +19476,14 @@
       <c r="B180" s="8">
         <v>461</v>
       </c>
-      <c r="C180" s="8" t="s">
-        <v>578</v>
+      <c r="C180" s="2" t="s">
+        <v>575</v>
       </c>
       <c r="D180" s="22" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E180" s="12" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F180" s="2" t="s">
         <v>4</v>
@@ -17754,21 +19492,27 @@
         <v>42743</v>
       </c>
       <c r="H180" s="8" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="T180" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:34" ht="232" x14ac:dyDescent="0.35">
       <c r="A181" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B181" s="8">
         <v>477</v>
       </c>
-      <c r="C181" s="8" t="s">
-        <v>581</v>
+      <c r="C181" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D181" s="22" t="s">
+        <v>633</v>
+      </c>
+      <c r="E181" s="13" t="s">
+        <v>634</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>81</v>
@@ -17777,7 +19521,7 @@
         <v>42743</v>
       </c>
       <c r="H181" s="8" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="182" spans="1:34" ht="72.5" x14ac:dyDescent="0.35">
@@ -17787,14 +19531,14 @@
       <c r="B182" s="2">
         <v>342</v>
       </c>
-      <c r="C182" s="8" t="s">
-        <v>456</v>
+      <c r="C182" s="2" t="s">
+        <v>453</v>
       </c>
       <c r="D182" s="22" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E182" s="13" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>81</v>
@@ -17813,14 +19557,14 @@
       <c r="B183" s="8">
         <v>151</v>
       </c>
-      <c r="C183" s="8" t="s">
+      <c r="C183" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="D183" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="E183" s="13" t="s">
         <v>588</v>
-      </c>
-      <c r="D183" s="22" t="s">
-        <v>592</v>
-      </c>
-      <c r="E183" s="13" t="s">
-        <v>591</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>127</v>
@@ -17829,7 +19573,7 @@
         <v>42743</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="O183" s="8" t="s">
         <v>5</v>
@@ -17842,14 +19586,14 @@
       <c r="B184" s="8">
         <v>186</v>
       </c>
-      <c r="C184" s="8" t="s">
+      <c r="C184" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="D184" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="D184" s="22" t="s">
+      <c r="E184" s="13" t="s">
         <v>596</v>
-      </c>
-      <c r="E184" s="13" t="s">
-        <v>599</v>
       </c>
       <c r="F184" s="2" t="s">
         <v>4</v>
@@ -17858,7 +19602,7 @@
         <v>42377</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="I184" s="8" t="s">
         <v>5</v>
@@ -17871,14 +19615,14 @@
       <c r="B185" s="8">
         <v>49</v>
       </c>
-      <c r="C185" s="8" t="s">
-        <v>602</v>
+      <c r="C185" s="2" t="s">
+        <v>598</v>
       </c>
       <c r="D185" s="22" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E185" s="13" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F185" s="2" t="s">
         <v>32</v>
@@ -17887,7 +19631,7 @@
         <v>42377</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="J185" s="8" t="s">
         <v>5</v>
@@ -17903,14 +19647,14 @@
       <c r="B186" s="8">
         <v>382</v>
       </c>
-      <c r="C186" s="8" t="s">
-        <v>611</v>
+      <c r="C186" s="2" t="s">
+        <v>607</v>
       </c>
       <c r="D186" s="22" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E186" s="13" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="F186" s="2" t="s">
         <v>4</v>
@@ -17935,14 +19679,14 @@
       <c r="B187" s="8">
         <v>398</v>
       </c>
-      <c r="C187" s="8" t="s">
-        <v>613</v>
+      <c r="C187" s="2" t="s">
+        <v>609</v>
       </c>
       <c r="D187" s="22" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="E187" s="13" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="F187" s="2" t="s">
         <v>4</v>
@@ -17951,7 +19695,7 @@
         <v>42743</v>
       </c>
       <c r="H187" s="8" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="AF187" s="8" t="s">
         <v>5</v>
@@ -17960,20 +19704,418 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:34" ht="174" x14ac:dyDescent="0.35">
-      <c r="A190" s="2" t="s">
+    <row r="188" spans="1:34" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A188" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B188" s="8">
+        <v>11</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="D188" s="22" t="s">
+        <v>614</v>
+      </c>
+      <c r="E188" s="13" t="s">
+        <v>612</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G188" s="9">
+        <v>42744</v>
+      </c>
+      <c r="H188" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="K188" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L188" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:34" ht="228" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A189" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B189" s="8">
+        <v>42</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="D189" s="22" t="s">
+        <v>617</v>
+      </c>
+      <c r="E189" s="17" t="s">
+        <v>616</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G189" s="9">
+        <v>42744</v>
+      </c>
+      <c r="H189" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="K189" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L189" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA189" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:34" ht="270.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B190" s="8">
+        <v>80</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="D190" s="22" t="s">
+        <v>620</v>
+      </c>
+      <c r="E190" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G190" s="9">
+        <v>42745</v>
+      </c>
+      <c r="H190" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="K190" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L190" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:34" ht="206.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A191" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B191" s="8">
+        <v>81</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D191" s="22" t="s">
+        <v>629</v>
+      </c>
+      <c r="E191" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="F191" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G191" s="9">
+        <v>42745</v>
+      </c>
+      <c r="H191" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="L191" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X191" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:34" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A192" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B192" s="8">
+        <v>33</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="D192" s="22" t="s">
+        <v>627</v>
+      </c>
+      <c r="E192" s="13" t="s">
+        <v>626</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G192" s="9">
+        <v>42745</v>
+      </c>
+      <c r="H192" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="L192" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="X192" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:33" ht="174" x14ac:dyDescent="0.35">
+      <c r="A193" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B193" s="8">
+        <v>54</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D193" s="22" t="s">
+        <v>631</v>
+      </c>
+      <c r="E193" s="13" t="s">
+        <v>632</v>
+      </c>
+      <c r="F193" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G193" s="9">
+        <v>42745</v>
+      </c>
+      <c r="H193" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="L193" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:33" ht="174" x14ac:dyDescent="0.35">
+      <c r="A194" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B194" s="8">
+        <v>59</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="D194" s="22" t="s">
+        <v>636</v>
+      </c>
+      <c r="E194" s="12" t="s">
+        <v>637</v>
+      </c>
+      <c r="F194" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G194" s="9">
+        <v>42745</v>
+      </c>
+      <c r="L194" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:33" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A195" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B195" s="8">
+        <v>73</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="D195" s="22" t="s">
+        <v>639</v>
+      </c>
+      <c r="E195" s="13" t="s">
+        <v>640</v>
+      </c>
+      <c r="F195" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G195" s="9">
+        <v>42745</v>
+      </c>
+      <c r="H195" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="L195" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:33" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A196" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B196" s="8">
+        <v>289</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="D196" s="22" t="s">
+        <v>651</v>
+      </c>
+      <c r="E196" s="13" t="s">
+        <v>652</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G196" s="9">
+        <v>42746</v>
+      </c>
+      <c r="H196" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="L196" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="T196" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:33" ht="116" x14ac:dyDescent="0.35">
+      <c r="A197" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B197" s="8">
+        <v>228</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="D197" s="22" t="s">
+        <v>657</v>
+      </c>
+      <c r="E197" s="13" t="s">
+        <v>658</v>
+      </c>
+      <c r="F197" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G197" s="9">
+        <v>42746</v>
+      </c>
+      <c r="H197" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="L197" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:33" ht="145" x14ac:dyDescent="0.35">
+      <c r="A198" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B198" s="8">
+        <v>209</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D198" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="E198" s="13" t="s">
+        <v>661</v>
+      </c>
+      <c r="F198" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G198" s="9">
+        <v>42746</v>
+      </c>
+      <c r="H198" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="K198" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L198" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:33" ht="232" x14ac:dyDescent="0.35">
+      <c r="A199" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B190" s="2">
+      <c r="B199" s="8">
+        <v>448</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="D199" s="22" t="s">
+        <v>664</v>
+      </c>
+      <c r="E199" s="13" t="s">
+        <v>666</v>
+      </c>
+      <c r="F199" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G199" s="9">
+        <v>42746</v>
+      </c>
+      <c r="H199" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="L199" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:33" ht="203" x14ac:dyDescent="0.35">
+      <c r="A200" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B200" s="8">
+        <v>455</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="D200" s="22" t="s">
+        <v>669</v>
+      </c>
+      <c r="E200" s="13" t="s">
+        <v>668</v>
+      </c>
+      <c r="F200" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G200" s="9">
+        <v>42746</v>
+      </c>
+      <c r="L200" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG200" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:33" ht="174" x14ac:dyDescent="0.35">
+      <c r="A203" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B203" s="2">
         <v>405</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C203" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="D190" s="22" t="s">
+      <c r="D203" s="22" t="s">
         <v>414</v>
       </c>
-      <c r="F190" s="22"/>
+      <c r="F203" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18013,7 +20155,7 @@
         <v>311</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="58" x14ac:dyDescent="0.35">
@@ -18039,10 +20181,10 @@
         <v>256</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="145" x14ac:dyDescent="0.35">
@@ -18064,10 +20206,10 @@
         <v>313</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
@@ -18137,7 +20279,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>16</v>
@@ -18145,10 +20287,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B8" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -18159,11 +20301,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18189,60 +20331,68 @@
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>434</v>
+        <v>646</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>428</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>429</v>
+        <v>650</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>648</v>
       </c>
     </row>
   </sheetData>
@@ -18252,22 +20402,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18278,34 +20439,50 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>600</v>
+        <v>656</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B3" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="174" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>608</v>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>